<commit_message>
RMSE for yield and t_stamp adjustment
- rmse calculation for yield
- t_stamp adjustment for the data in mechanistic folder
</commit_message>
<xml_diff>
--- a/exposan/pm2_ecorecover/data/dynamic_simul_result_calibration.xlsx
+++ b/exposan/pm2_ecorecover/data/dynamic_simul_result_calibration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Downloads\EXPOsan\exposan\pm2_ecorecover\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{904F1481-6EDE-48E0-91AF-6FDF1488E6C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985C642C-754F-4E63-B05B-204235C2E47C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{DEEFF93F-8712-407E-800A-077FF6958EEC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>t_stamp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,6 +36,14 @@
   </si>
   <si>
     <t>SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yield_1d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_stamp_yield</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -401,15 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47DDD832-617E-423B-B3BC-9FD3F4E9EB72}">
-  <dimension ref="A1:C252"/>
+  <dimension ref="A1:E252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A252"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,8 +427,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -430,8 +444,14 @@
       <c r="C2" s="1">
         <v>0.35744153755741681</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E2">
+        <v>141.22641287052892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -441,8 +461,14 @@
       <c r="C3" s="1">
         <v>1.107531976471491E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+      <c r="E3">
+        <v>135.97279294533516</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -452,8 +478,14 @@
       <c r="C4" s="1">
         <v>8.023750326828151E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1.3</v>
+      </c>
+      <c r="E4">
+        <v>137.25611599582237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.3</v>
       </c>
@@ -463,8 +495,14 @@
       <c r="C5" s="1">
         <v>8.3368790863734953E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>1.4</v>
+      </c>
+      <c r="E5">
+        <v>141.4937078208886</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.4</v>
       </c>
@@ -474,8 +512,14 @@
       <c r="C6" s="1">
         <v>8.4525318869409678E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>1.5</v>
+      </c>
+      <c r="E6">
+        <v>146.22981559997456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -485,8 +529,14 @@
       <c r="C7" s="1">
         <v>8.2427629558514404E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>1.6</v>
+      </c>
+      <c r="E7">
+        <v>155.19516202553595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.60000000000000009</v>
       </c>
@@ -496,8 +546,14 @@
       <c r="C8" s="1">
         <v>8.047608090998748E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>1.7</v>
+      </c>
+      <c r="E8">
+        <v>164.48641289040361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.70000000000000007</v>
       </c>
@@ -507,8 +563,14 @@
       <c r="C9" s="1">
         <v>7.6928155733528526E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>1.8</v>
+      </c>
+      <c r="E9">
+        <v>162.94445964495671</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.8</v>
       </c>
@@ -518,8 +580,14 @@
       <c r="C10" s="1">
         <v>7.5928288121893429E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>1.9</v>
+      </c>
+      <c r="E10">
+        <v>166.38433793495579</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.9</v>
       </c>
@@ -529,8 +597,14 @@
       <c r="C11" s="1">
         <v>7.7011487317907162E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>171.90915255790085</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -540,8 +614,14 @@
       <c r="C12" s="1">
         <v>7.7124903485505016E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>2.1</v>
+      </c>
+      <c r="E12">
+        <v>185.10118651133465</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1.1000000000000001</v>
       </c>
@@ -551,8 +631,14 @@
       <c r="C13" s="1">
         <v>7.6850542823217946E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E13">
+        <v>194.07285149384563</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1.2</v>
       </c>
@@ -562,8 +648,14 @@
       <c r="C14" s="1">
         <v>7.5907843687077828E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E14">
+        <v>204.71501041834455</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1.3</v>
       </c>
@@ -573,8 +665,14 @@
       <c r="C15" s="1">
         <v>7.4713145778358223E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>2.4</v>
+      </c>
+      <c r="E15">
+        <v>218.07116024736308</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1.4</v>
       </c>
@@ -584,8 +682,14 @@
       <c r="C16" s="1">
         <v>7.4172540833685281E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>2.5</v>
+      </c>
+      <c r="E16">
+        <v>238.31941931582114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1.5</v>
       </c>
@@ -595,8 +699,14 @@
       <c r="C17" s="1">
         <v>7.1545651875343577E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>2.6</v>
+      </c>
+      <c r="E17">
+        <v>272.09624752272452</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1.6</v>
       </c>
@@ -606,8 +716,14 @@
       <c r="C18" s="1">
         <v>6.8176199738561108E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>2.7</v>
+      </c>
+      <c r="E18">
+        <v>307.41925825383117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1.7</v>
       </c>
@@ -617,8 +733,14 @@
       <c r="C19" s="1">
         <v>6.4030155962494471E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>2.8</v>
+      </c>
+      <c r="E19">
+        <v>311.20108197779354</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1.8</v>
       </c>
@@ -628,8 +750,14 @@
       <c r="C20" s="1">
         <v>6.1844623865160526E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>2.9</v>
+      </c>
+      <c r="E20">
+        <v>316.16888749769345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1.9</v>
       </c>
@@ -639,8 +767,14 @@
       <c r="C21" s="1">
         <v>5.890199985453818E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>326.15154922902803</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -650,8 +784,14 @@
       <c r="C22" s="1">
         <v>5.6469543849011847E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>3.1</v>
+      </c>
+      <c r="E22">
+        <v>324.02324436213377</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2.1</v>
       </c>
@@ -661,8 +801,14 @@
       <c r="C23" s="1">
         <v>5.3266579662909798E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>3.2</v>
+      </c>
+      <c r="E23">
+        <v>315.57106974593427</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2.2000000000000002</v>
       </c>
@@ -672,8 +818,14 @@
       <c r="C24" s="1">
         <v>4.9245021171890301E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>3.3</v>
+      </c>
+      <c r="E24">
+        <v>305.0056768948071</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2.2999999999999998</v>
       </c>
@@ -683,8 +835,14 @@
       <c r="C25" s="1">
         <v>4.4682823813590924E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>3.4</v>
+      </c>
+      <c r="E25">
+        <v>296.98411351130693</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2.4</v>
       </c>
@@ -694,8 +852,14 @@
       <c r="C26" s="1">
         <v>4.1120777190817859E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>3.5</v>
+      </c>
+      <c r="E26">
+        <v>290.32990663325063</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2.5</v>
       </c>
@@ -705,8 +869,14 @@
       <c r="C27" s="1">
         <v>3.900444179544525E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>3.6</v>
+      </c>
+      <c r="E27">
+        <v>281.10983535961992</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2.6</v>
       </c>
@@ -716,8 +886,14 @@
       <c r="C28" s="1">
         <v>3.662563688739968E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>3.7</v>
+      </c>
+      <c r="E28">
+        <v>263.79042643133266</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2.7</v>
       </c>
@@ -727,8 +903,14 @@
       <c r="C29" s="1">
         <v>3.5054778851214912E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>3.8</v>
+      </c>
+      <c r="E29">
+        <v>217.35976430814989</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2.8</v>
       </c>
@@ -738,8 +920,14 @@
       <c r="C30" s="1">
         <v>3.4563613546098049E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>3.9</v>
+      </c>
+      <c r="E30">
+        <v>185.49583065482707</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2.9</v>
       </c>
@@ -749,8 +937,14 @@
       <c r="C31" s="1">
         <v>3.5341997975597739E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>164.67647430927929</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -760,8 +954,14 @@
       <c r="C32" s="1">
         <v>3.6180510852257151E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>4.1000000000000014</v>
+      </c>
+      <c r="E32">
+        <v>143.97381475632523</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3.1</v>
       </c>
@@ -771,8 +971,14 @@
       <c r="C33" s="1">
         <v>3.963679945281906E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <v>4.2</v>
+      </c>
+      <c r="E33">
+        <v>133.95044793283728</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3.2</v>
       </c>
@@ -782,8 +988,14 @@
       <c r="C34" s="1">
         <v>4.1607249923814628E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <v>4.3</v>
+      </c>
+      <c r="E34">
+        <v>128.69920570803458</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3.3</v>
       </c>
@@ -793,8 +1005,14 @@
       <c r="C35" s="1">
         <v>4.4811730158857681E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E35">
+        <v>125.82675414951444</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>3.4</v>
       </c>
@@ -804,8 +1022,14 @@
       <c r="C36" s="1">
         <v>4.9060457617201708E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <v>4.5</v>
+      </c>
+      <c r="E36">
+        <v>122.31902451577163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>3.5</v>
       </c>
@@ -815,8 +1039,14 @@
       <c r="C37" s="1">
         <v>5.375602114115423E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37">
+        <v>4.6000000000000014</v>
+      </c>
+      <c r="E37">
+        <v>119.08849859686953</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>3.6</v>
       </c>
@@ -826,8 +1056,14 @@
       <c r="C38" s="1">
         <v>5.7965711613269539E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <v>4.7</v>
+      </c>
+      <c r="E38">
+        <v>107.75993290630599</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3.7</v>
       </c>
@@ -837,8 +1073,14 @@
       <c r="C39" s="1">
         <v>6.1668751874600428E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39">
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="E39">
+        <v>80.454469551759615</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>3.8</v>
       </c>
@@ -848,8 +1090,14 @@
       <c r="C40" s="1">
         <v>6.7841741523916137E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E40">
+        <v>70.6610342144795</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>3.9</v>
       </c>
@@ -859,8 +1107,14 @@
       <c r="C41" s="1">
         <v>7.3934642554173398E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41">
+        <v>5</v>
+      </c>
+      <c r="E41">
+        <v>69.105060705339895</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>4</v>
       </c>
@@ -870,8 +1124,14 @@
       <c r="C42" s="1">
         <v>8.0319126961436119E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42">
+        <v>5.1000000000000014</v>
+      </c>
+      <c r="E42">
+        <v>67.769369182296799</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4.1000000000000014</v>
       </c>
@@ -881,8 +1141,14 @@
       <c r="C43" s="1">
         <v>8.7566441485514932E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43">
+        <v>5.2</v>
+      </c>
+      <c r="E43">
+        <v>66.622472229871377</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>4.2</v>
       </c>
@@ -892,8 +1158,14 @@
       <c r="C44" s="1">
         <v>9.340020468893314E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44">
+        <v>5.3000000000000007</v>
+      </c>
+      <c r="E44">
+        <v>65.734720727098164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>4.3</v>
       </c>
@@ -903,8 +1175,14 @@
       <c r="C45" s="1">
         <v>1.005687504009666E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45">
+        <v>5.4</v>
+      </c>
+      <c r="E45">
+        <v>66.91647524561543</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>4.4000000000000004</v>
       </c>
@@ -914,8 +1192,14 @@
       <c r="C46" s="1">
         <v>1.056710418044126E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <v>5.5</v>
+      </c>
+      <c r="E46">
+        <v>69.792775866637314</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4.5</v>
       </c>
@@ -925,8 +1209,14 @@
       <c r="C47" s="1">
         <v>1.1050850441609439E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <v>5.6000000000000014</v>
+      </c>
+      <c r="E47">
+        <v>71.999558753876386</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>4.6000000000000014</v>
       </c>
@@ -936,8 +1226,14 @@
       <c r="C48" s="1">
         <v>1.1393393895568831E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>5.7</v>
+      </c>
+      <c r="E48">
+        <v>69.889997832841473</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4.7</v>
       </c>
@@ -947,8 +1243,14 @@
       <c r="C49" s="1">
         <v>1.166064289197348E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="E49">
+        <v>62.205462418638056</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>4.8000000000000007</v>
       </c>
@@ -958,8 +1260,14 @@
       <c r="C50" s="1">
         <v>1.199332966342577E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <v>5.9</v>
+      </c>
+      <c r="E50">
+        <v>58.996395382408672</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>4.9000000000000004</v>
       </c>
@@ -969,8 +1277,14 @@
       <c r="C51" s="1">
         <v>1.226872553654202E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51">
+        <v>6</v>
+      </c>
+      <c r="E51">
+        <v>59.091189459017215</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>5</v>
       </c>
@@ -980,8 +1294,14 @@
       <c r="C52" s="1">
         <v>1.2707943516759209E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <v>6.1000000000000014</v>
+      </c>
+      <c r="E52">
+        <v>59.297671256470601</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5.1000000000000014</v>
       </c>
@@ -991,8 +1311,14 @@
       <c r="C53" s="1">
         <v>1.3117618006091E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53">
+        <v>6.2</v>
+      </c>
+      <c r="E53">
+        <v>59.666896195248796</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>5.2</v>
       </c>
@@ -1002,8 +1328,14 @@
       <c r="C54" s="1">
         <v>1.324983839921591E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54">
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="E54">
+        <v>60.169494063175463</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>5.3000000000000007</v>
       </c>
@@ -1013,8 +1345,14 @@
       <c r="C55" s="1">
         <v>1.364164342781549E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55">
+        <v>6.4</v>
+      </c>
+      <c r="E55">
+        <v>62.273426130964296</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>5.4</v>
       </c>
@@ -1024,8 +1362,14 @@
       <c r="C56" s="1">
         <v>1.369136083747537E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56">
+        <v>6.5</v>
+      </c>
+      <c r="E56">
+        <v>64.850657243796263</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>5.5</v>
       </c>
@@ -1035,8 +1379,14 @@
       <c r="C57" s="1">
         <v>1.391303899136772E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <v>6.6000000000000014</v>
+      </c>
+      <c r="E57">
+        <v>66.648301432291248</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>5.6000000000000014</v>
       </c>
@@ -1046,8 +1396,14 @@
       <c r="C58" s="1">
         <v>1.3763069438431389E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58">
+        <v>6.7</v>
+      </c>
+      <c r="E58">
+        <v>66.326706835516902</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>5.7</v>
       </c>
@@ -1057,8 +1413,14 @@
       <c r="C59" s="1">
         <v>1.387122135430891E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="E59">
+        <v>61.901482579563634</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>5.8000000000000007</v>
       </c>
@@ -1068,8 +1430,14 @@
       <c r="C60" s="1">
         <v>1.385835732877426E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>6.9</v>
+      </c>
+      <c r="E60">
+        <v>60.457148802318507</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>5.9</v>
       </c>
@@ -1079,8 +1447,14 @@
       <c r="C61" s="1">
         <v>1.4215790718244491E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>7</v>
+      </c>
+      <c r="E61">
+        <v>62.838532845573553</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>6</v>
       </c>
@@ -1090,8 +1464,14 @@
       <c r="C62" s="1">
         <v>1.4306328030382891E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62">
+        <v>7.1000000000000014</v>
+      </c>
+      <c r="E62">
+        <v>66.161927305941902</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>6.1000000000000014</v>
       </c>
@@ -1101,8 +1481,14 @@
       <c r="C63" s="1">
         <v>1.465699042511567E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63">
+        <v>7.2</v>
+      </c>
+      <c r="E63">
+        <v>69.524153233279534</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>6.2</v>
       </c>
@@ -1112,8 +1498,14 @@
       <c r="C64" s="1">
         <v>1.4793210369891259E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64">
+        <v>7.3000000000000007</v>
+      </c>
+      <c r="E64">
+        <v>72.138253257486539</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>6.3000000000000007</v>
       </c>
@@ -1123,8 +1515,14 @@
       <c r="C65" s="1">
         <v>1.503102911195551E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65">
+        <v>7.4</v>
+      </c>
+      <c r="E65">
+        <v>75.030372357463406</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>6.4</v>
       </c>
@@ -1134,8 +1532,14 @@
       <c r="C66" s="1">
         <v>1.5295859825186719E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <v>7.5</v>
+      </c>
+      <c r="E66">
+        <v>78.366202266904381</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>6.5</v>
       </c>
@@ -1145,8 +1549,14 @@
       <c r="C67" s="1">
         <v>1.527187094526922E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <v>7.6000000000000014</v>
+      </c>
+      <c r="E67">
+        <v>80.690828485220308</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>6.6000000000000014</v>
       </c>
@@ -1156,8 +1566,14 @@
       <c r="C68" s="1">
         <v>1.5306904098264389E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>7.7</v>
+      </c>
+      <c r="E68">
+        <v>84.527857271848703</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>6.7</v>
       </c>
@@ -1167,8 +1583,14 @@
       <c r="C69" s="1">
         <v>1.5299679827600981E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <v>7.8000000000000007</v>
+      </c>
+      <c r="E69">
+        <v>79.56130898264756</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>6.8000000000000007</v>
       </c>
@@ -1178,8 +1600,14 @@
       <c r="C70" s="1">
         <v>1.5198612509803521E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70">
+        <v>7.9</v>
+      </c>
+      <c r="E70">
+        <v>71.996111088716148</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>6.9</v>
       </c>
@@ -1189,8 +1617,14 @@
       <c r="C71" s="1">
         <v>1.528280404432324E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>8</v>
+      </c>
+      <c r="E71">
+        <v>67.896267524560074</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>7</v>
       </c>
@@ -1200,8 +1634,14 @@
       <c r="C72" s="1">
         <v>1.5302512144562141E-2</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72">
+        <v>8.1</v>
+      </c>
+      <c r="E72">
+        <v>66.181918062494347</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>7.1000000000000014</v>
       </c>
@@ -1211,8 +1651,14 @@
       <c r="C73" s="1">
         <v>1.5202374297606919E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <v>8.2000000000000011</v>
+      </c>
+      <c r="E73">
+        <v>64.035443585099245</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>7.2</v>
       </c>
@@ -1222,8 +1668,14 @@
       <c r="C74" s="1">
         <v>1.5050079679233139E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E74">
+        <v>62.062452959333221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>7.3000000000000007</v>
       </c>
@@ -1233,8 +1685,14 @@
       <c r="C75" s="1">
         <v>1.521206802512476E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>8.4</v>
+      </c>
+      <c r="E75">
+        <v>62.509860016672995</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>7.4</v>
       </c>
@@ -1244,8 +1702,14 @@
       <c r="C76" s="1">
         <v>1.554036744227931E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>8.5</v>
+      </c>
+      <c r="E76">
+        <v>64.361445104550242</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>7.5</v>
       </c>
@@ -1255,8 +1719,14 @@
       <c r="C77" s="1">
         <v>1.557397797271105E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77">
+        <v>8.6</v>
+      </c>
+      <c r="E77">
+        <v>67.97017108583151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>7.6000000000000014</v>
       </c>
@@ -1266,8 +1736,14 @@
       <c r="C78" s="1">
         <v>1.579028696060486E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78">
+        <v>8.7000000000000011</v>
+      </c>
+      <c r="E78">
+        <v>73.756488747295904</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>7.7</v>
       </c>
@@ -1277,8 +1753,14 @@
       <c r="C79" s="1">
         <v>1.544228227985996E-2</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E79">
+        <v>69.104290423400585</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>7.8000000000000007</v>
       </c>
@@ -1288,8 +1770,14 @@
       <c r="C80" s="1">
         <v>1.5649686977813351E-2</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>8.9</v>
+      </c>
+      <c r="E80">
+        <v>67.356434819572897</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>7.9</v>
       </c>
@@ -1299,8 +1787,14 @@
       <c r="C81" s="1">
         <v>1.5980002786042509E-2</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>9</v>
+      </c>
+      <c r="E81">
+        <v>72.006876520816348</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>8</v>
       </c>
@@ -1310,8 +1804,14 @@
       <c r="C82" s="1">
         <v>1.6729880685912229E-2</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>9.1</v>
+      </c>
+      <c r="E82">
+        <v>76.912306483218003</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>8.1</v>
       </c>
@@ -1321,8 +1821,14 @@
       <c r="C83" s="1">
         <v>1.6759911977767449E-2</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>9.2000000000000011</v>
+      </c>
+      <c r="E83">
+        <v>78.595175802044309</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>8.2000000000000011</v>
       </c>
@@ -1332,8 +1838,14 @@
       <c r="C84" s="1">
         <v>1.67846543111933E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E84">
+        <v>80.106090167518261</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>8.3000000000000007</v>
       </c>
@@ -1343,8 +1855,14 @@
       <c r="C85" s="1">
         <v>1.6594358724505359E-2</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>9.4</v>
+      </c>
+      <c r="E85">
+        <v>83.524617936634399</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>8.4</v>
       </c>
@@ -1354,8 +1872,14 @@
       <c r="C86" s="1">
         <v>1.6344963736168679E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>9.5</v>
+      </c>
+      <c r="E86">
+        <v>88.966936865417466</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>8.5</v>
       </c>
@@ -1365,8 +1889,14 @@
       <c r="C87" s="1">
         <v>1.6002392676923591E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="E87">
+        <v>93.385143939669902</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>8.6</v>
       </c>
@@ -1376,8 +1906,14 @@
       <c r="C88" s="1">
         <v>1.552642384107283E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>9.7000000000000011</v>
+      </c>
+      <c r="E88">
+        <v>97.714759568979829</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>8.7000000000000011</v>
       </c>
@@ -1387,8 +1923,14 @@
       <c r="C89" s="1">
         <v>1.457597872810504E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E89">
+        <v>89.837050977472032</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>8.8000000000000007</v>
       </c>
@@ -1398,8 +1940,14 @@
       <c r="C90" s="1">
         <v>1.4167911938584561E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90">
+        <v>9.9</v>
+      </c>
+      <c r="E90">
+        <v>84.685777993895087</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>8.9</v>
       </c>
@@ -1409,8 +1957,14 @@
       <c r="C91" s="1">
         <v>1.39619055632788E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <v>10</v>
+      </c>
+      <c r="E91">
+        <v>84.276444503853838</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>9</v>
       </c>
@@ -1420,8 +1974,14 @@
       <c r="C92" s="1">
         <v>1.371319055641233E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92">
+        <v>10.1</v>
+      </c>
+      <c r="E92">
+        <v>82.39011785191704</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>9.1</v>
       </c>
@@ -1431,8 +1991,14 @@
       <c r="C93" s="1">
         <v>1.3410869000320491E-2</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E93">
+        <v>82.192089179606214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>9.2000000000000011</v>
       </c>
@@ -1442,8 +2008,14 @@
       <c r="C94" s="1">
         <v>1.309901987120321E-2</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94">
+        <v>10.3</v>
+      </c>
+      <c r="E94">
+        <v>82.473039790810247</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>9.3000000000000007</v>
       </c>
@@ -1453,8 +2025,14 @@
       <c r="C95" s="1">
         <v>1.2785479007028099E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95">
+        <v>10.4</v>
+      </c>
+      <c r="E95">
+        <v>83.736316238605241</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>9.4</v>
       </c>
@@ -1464,8 +2042,14 @@
       <c r="C96" s="1">
         <v>1.236175574158252E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D96">
+        <v>10.5</v>
+      </c>
+      <c r="E96">
+        <v>85.188818895842346</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>9.5</v>
       </c>
@@ -1475,8 +2059,14 @@
       <c r="C97" s="1">
         <v>1.1823278127276749E-2</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D97">
+        <v>10.6</v>
+      </c>
+      <c r="E97">
+        <v>84.269834050745573</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>9.6000000000000014</v>
       </c>
@@ -1486,8 +2076,14 @@
       <c r="C98" s="1">
         <v>1.139245045375299E-2</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D98">
+        <v>10.7</v>
+      </c>
+      <c r="E98">
+        <v>81.745703681267173</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>9.7000000000000011</v>
       </c>
@@ -1497,8 +2093,14 @@
       <c r="C99" s="1">
         <v>1.0919789190071199E-2</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D99">
+        <v>10.8</v>
+      </c>
+      <c r="E99">
+        <v>73.31680498787108</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>9.8000000000000007</v>
       </c>
@@ -1508,8 +2110,14 @@
       <c r="C100" s="1">
         <v>1.0540817049596189E-2</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D100">
+        <v>10.9</v>
+      </c>
+      <c r="E100">
+        <v>73.024892627670155</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>9.9</v>
       </c>
@@ -1519,8 +2127,14 @@
       <c r="C101" s="1">
         <v>1.025390064694965E-2</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D101">
+        <v>11</v>
+      </c>
+      <c r="E101">
+        <v>76.171723874362442</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>10</v>
       </c>
@@ -1530,8 +2144,14 @@
       <c r="C102" s="1">
         <v>9.9826400208533686E-3</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D102">
+        <v>11.1</v>
+      </c>
+      <c r="E102">
+        <v>79.731468800898838</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>10.1</v>
       </c>
@@ -1541,8 +2161,14 @@
       <c r="C103" s="1">
         <v>9.6883819608733143E-3</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D103">
+        <v>11.2</v>
+      </c>
+      <c r="E103">
+        <v>84.926117407681105</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>10.199999999999999</v>
       </c>
@@ -1552,8 +2178,14 @@
       <c r="C104" s="1">
         <v>9.2910202099324244E-3</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D104">
+        <v>11.3</v>
+      </c>
+      <c r="E104">
+        <v>88.196861862918013</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>10.3</v>
       </c>
@@ -1563,8 +2195,14 @@
       <c r="C105" s="1">
         <v>8.8389841353768046E-3</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D105">
+        <v>11.4</v>
+      </c>
+      <c r="E105">
+        <v>93.162862203673726</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>10.4</v>
       </c>
@@ -1574,8 +2212,14 @@
       <c r="C106" s="1">
         <v>8.3701684432845314E-3</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D106">
+        <v>11.5</v>
+      </c>
+      <c r="E106">
+        <v>103.4426825283621</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>10.5</v>
       </c>
@@ -1585,8 +2229,14 @@
       <c r="C107" s="1">
         <v>8.0773493100987238E-3</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D107">
+        <v>11.6</v>
+      </c>
+      <c r="E107">
+        <v>109.03260580205861</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>10.6</v>
       </c>
@@ -1596,8 +2246,14 @@
       <c r="C108" s="1">
         <v>7.7857282493948247E-3</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D108">
+        <v>11.7</v>
+      </c>
+      <c r="E108">
+        <v>113.72818004229948</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>10.7</v>
       </c>
@@ -1607,8 +2263,14 @@
       <c r="C109" s="1">
         <v>7.4779006302009791E-3</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D109">
+        <v>11.8</v>
+      </c>
+      <c r="E109">
+        <v>115.00859453318331</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>10.8</v>
       </c>
@@ -1618,8 +2280,14 @@
       <c r="C110" s="1">
         <v>7.2986977702901128E-3</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D110">
+        <v>11.9</v>
+      </c>
+      <c r="E110">
+        <v>114.76792465710119</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>10.9</v>
       </c>
@@ -1629,8 +2297,14 @@
       <c r="C111" s="1">
         <v>7.1549567989567789E-3</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D111">
+        <v>12</v>
+      </c>
+      <c r="E111">
+        <v>115.17166502180503</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>11</v>
       </c>
@@ -1640,8 +2314,14 @@
       <c r="C112" s="1">
         <v>6.9610729085756969E-3</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D112">
+        <v>12.1</v>
+      </c>
+      <c r="E112">
+        <v>116.01924680569674</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>11.1</v>
       </c>
@@ -1651,8 +2331,14 @@
       <c r="C113" s="1">
         <v>6.7900989115672744E-3</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D113">
+        <v>12.2</v>
+      </c>
+      <c r="E113">
+        <v>116.58742112065853</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>11.2</v>
       </c>
@@ -1662,8 +2348,14 @@
       <c r="C114" s="1">
         <v>6.8278936740797597E-3</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D114">
+        <v>12.3</v>
+      </c>
+      <c r="E114">
+        <v>117.28985356508851</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>11.3</v>
       </c>
@@ -1673,8 +2365,14 @@
       <c r="C115" s="1">
         <v>6.6296016918297312E-3</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D115">
+        <v>12.4</v>
+      </c>
+      <c r="E115">
+        <v>121.21788906979003</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>11.4</v>
       </c>
@@ -1684,8 +2382,14 @@
       <c r="C116" s="1">
         <v>6.6811396618864224E-3</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D116">
+        <v>12.5</v>
+      </c>
+      <c r="E116">
+        <v>130.51844692658599</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>11.5</v>
       </c>
@@ -1695,8 +2399,14 @@
       <c r="C117" s="1">
         <v>6.5243756549859134E-3</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D117">
+        <v>12.6</v>
+      </c>
+      <c r="E117">
+        <v>135.70093781055797</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>11.6</v>
       </c>
@@ -1706,8 +2416,14 @@
       <c r="C118" s="1">
         <v>6.4405641662449113E-3</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D118">
+        <v>12.7</v>
+      </c>
+      <c r="E118">
+        <v>143.88913505087058</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>11.7</v>
       </c>
@@ -1717,8 +2433,14 @@
       <c r="C119" s="1">
         <v>6.4784934559068523E-3</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D119">
+        <v>12.8</v>
+      </c>
+      <c r="E119">
+        <v>145.26423136997519</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>11.8</v>
       </c>
@@ -1728,8 +2450,14 @@
       <c r="C120" s="1">
         <v>6.325693973864753E-3</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D120">
+        <v>12.9</v>
+      </c>
+      <c r="E120">
+        <v>141.00582242427657</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>11.9</v>
       </c>
@@ -1739,8 +2467,14 @@
       <c r="C121" s="1">
         <v>6.3407840360676336E-3</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D121">
+        <v>13</v>
+      </c>
+      <c r="E121">
+        <v>140.58004266612076</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>12</v>
       </c>
@@ -1750,8 +2484,14 @@
       <c r="C122" s="1">
         <v>6.4335562604397418E-3</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D122">
+        <v>13.1</v>
+      </c>
+      <c r="E122">
+        <v>139.85438078728146</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>12.1</v>
       </c>
@@ -1761,8 +2501,14 @@
       <c r="C123" s="1">
         <v>6.2362993685006994E-3</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D123">
+        <v>13.2</v>
+      </c>
+      <c r="E123">
+        <v>138.42919754476924</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>12.2</v>
       </c>
@@ -1772,8 +2518,14 @@
       <c r="C124" s="1">
         <v>6.3025833835089872E-3</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D124">
+        <v>13.3</v>
+      </c>
+      <c r="E124">
+        <v>136.75807144930806</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>12.3</v>
       </c>
@@ -1783,8 +2535,14 @@
       <c r="C125" s="1">
         <v>6.3887410656872931E-3</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D125">
+        <v>13.4</v>
+      </c>
+      <c r="E125">
+        <v>136.33096750496463</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>12.4</v>
       </c>
@@ -1794,8 +2552,14 @@
       <c r="C126" s="1">
         <v>6.1514519382426646E-3</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D126">
+        <v>13.5</v>
+      </c>
+      <c r="E126">
+        <v>138.49194783720057</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>12.5</v>
       </c>
@@ -1805,8 +2569,14 @@
       <c r="C127" s="1">
         <v>6.1760566090801623E-3</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D127">
+        <v>13.6</v>
+      </c>
+      <c r="E127">
+        <v>136.93572900130602</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>12.6</v>
       </c>
@@ -1816,8 +2586,14 @@
       <c r="C128" s="1">
         <v>5.9427329344435391E-3</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D128">
+        <v>13.7</v>
+      </c>
+      <c r="E128">
+        <v>128.51617440954612</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>12.7</v>
       </c>
@@ -1827,8 +2603,14 @@
       <c r="C129" s="1">
         <v>5.9120398319980469E-3</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D129">
+        <v>13.8</v>
+      </c>
+      <c r="E129">
+        <v>115.34741378531913</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>12.8</v>
       </c>
@@ -1838,8 +2620,14 @@
       <c r="C130" s="1">
         <v>5.9660813791428836E-3</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D130">
+        <v>13.9</v>
+      </c>
+      <c r="E130">
+        <v>103.29798606292611</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>12.9</v>
       </c>
@@ -1849,8 +2637,14 @@
       <c r="C131" s="1">
         <v>6.0643245431174489E-3</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D131">
+        <v>14</v>
+      </c>
+      <c r="E131">
+        <v>101.11411408429127</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>13</v>
       </c>
@@ -1860,8 +2654,14 @@
       <c r="C132" s="1">
         <v>6.4882603096759724E-3</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D132">
+        <v>14.1</v>
+      </c>
+      <c r="E132">
+        <v>99.133180300042525</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>13.1</v>
       </c>
@@ -1871,8 +2671,14 @@
       <c r="C133" s="1">
         <v>6.6174701543940959E-3</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D133">
+        <v>14.2</v>
+      </c>
+      <c r="E133">
+        <v>97.597777919000819</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>13.2</v>
       </c>
@@ -1882,8 +2688,14 @@
       <c r="C134" s="1">
         <v>7.0581802478038164E-3</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D134">
+        <v>14.3</v>
+      </c>
+      <c r="E134">
+        <v>96.767501424670527</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>13.3</v>
       </c>
@@ -1893,8 +2705,14 @@
       <c r="C135" s="1">
         <v>7.505469630874553E-3</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D135">
+        <v>14.4</v>
+      </c>
+      <c r="E135">
+        <v>90.590565816466537</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>13.4</v>
       </c>
@@ -1904,8 +2722,14 @@
       <c r="C136" s="1">
         <v>7.9628694494917555E-3</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D136">
+        <v>14.5</v>
+      </c>
+      <c r="E136">
+        <v>84.297989863776309</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>13.5</v>
       </c>
@@ -1915,8 +2739,14 @@
       <c r="C137" s="1">
         <v>8.3662689757695204E-3</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D137">
+        <v>14.6</v>
+      </c>
+      <c r="E137">
+        <v>84.029982610536905</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>13.6</v>
       </c>
@@ -1926,8 +2756,14 @@
       <c r="C138" s="1">
         <v>8.7090820048649521E-3</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D138">
+        <v>14.7</v>
+      </c>
+      <c r="E138">
+        <v>96.256559634257712</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>13.7</v>
       </c>
@@ -1937,8 +2773,14 @@
       <c r="C139" s="1">
         <v>8.8313149896239087E-3</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D139">
+        <v>14.8</v>
+      </c>
+      <c r="E139">
+        <v>84.565967293903057</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>13.8</v>
       </c>
@@ -1948,8 +2790,14 @@
       <c r="C140" s="1">
         <v>9.2613684537093937E-3</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D140">
+        <v>14.9</v>
+      </c>
+      <c r="E140">
+        <v>74.633358258332606</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>13.9</v>
       </c>
@@ -1959,8 +2807,14 @@
       <c r="C141" s="1">
         <v>9.394103787288664E-3</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D141">
+        <v>15</v>
+      </c>
+      <c r="E141">
+        <v>69.869968783345342</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>14</v>
       </c>
@@ -1970,8 +2824,14 @@
       <c r="C142" s="1">
         <v>9.511823058263584E-3</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D142">
+        <v>15.1</v>
+      </c>
+      <c r="E142">
+        <v>67.557244698961711</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>14.1</v>
       </c>
@@ -1981,8 +2841,14 @@
       <c r="C143" s="1">
         <v>9.6211452826074871E-3</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D143">
+        <v>15.2</v>
+      </c>
+      <c r="E143">
+        <v>66.89781629080619</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>14.2</v>
       </c>
@@ -1992,8 +2858,14 @@
       <c r="C144" s="1">
         <v>9.3532182819897978E-3</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D144">
+        <v>15.3</v>
+      </c>
+      <c r="E144">
+        <v>66.141077419915774</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>14.3</v>
       </c>
@@ -2003,8 +2875,14 @@
       <c r="C145" s="1">
         <v>9.0710212460914617E-3</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D145">
+        <v>15.4</v>
+      </c>
+      <c r="E145">
+        <v>60.370957349435088</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>14.4</v>
       </c>
@@ -2014,8 +2892,14 @@
       <c r="C146" s="1">
         <v>8.7782520824585906E-3</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D146">
+        <v>15.5</v>
+      </c>
+      <c r="E146">
+        <v>60.831369924661139</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>14.5</v>
       </c>
@@ -2025,8 +2909,14 @@
       <c r="C147" s="1">
         <v>8.4919068041566879E-3</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D147">
+        <v>15.6</v>
+      </c>
+      <c r="E147">
+        <v>75.456023576206618</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>14.6</v>
       </c>
@@ -2036,8 +2926,14 @@
       <c r="C148" s="1">
         <v>8.1210191497048355E-3</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D148">
+        <v>15.7</v>
+      </c>
+      <c r="E148">
+        <v>94.887561618183454</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>14.7</v>
       </c>
@@ -2047,8 +2943,14 @@
       <c r="C149" s="1">
         <v>7.6084931948482036E-3</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D149">
+        <v>15.8</v>
+      </c>
+      <c r="E149">
+        <v>68.279684701028472</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>14.8</v>
       </c>
@@ -2058,8 +2960,14 @@
       <c r="C150" s="1">
         <v>7.2889628279638038E-3</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D150">
+        <v>15.9</v>
+      </c>
+      <c r="E150">
+        <v>71.193986598194329</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>14.9</v>
       </c>
@@ -2069,8 +2977,14 @@
       <c r="C151" s="1">
         <v>7.0976911323959524E-3</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D151">
+        <v>16</v>
+      </c>
+      <c r="E151">
+        <v>75.975192966038449</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>15</v>
       </c>
@@ -2080,8 +2994,14 @@
       <c r="C152" s="1">
         <v>7.2185703775433704E-3</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D152">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="E152">
+        <v>80.689754608043458</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>15.1</v>
       </c>
@@ -2091,8 +3011,14 @@
       <c r="C153">
         <v>7.2967599156929094E-3</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D153">
+        <v>16.2</v>
+      </c>
+      <c r="E153">
+        <v>82.799990795821728</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>15.2</v>
       </c>
@@ -2102,8 +3028,14 @@
       <c r="C154">
         <v>7.0160901062526638E-3</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D154">
+        <v>16.3</v>
+      </c>
+      <c r="E154">
+        <v>82.99556372043071</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>15.3</v>
       </c>
@@ -2113,8 +3045,14 @@
       <c r="C155">
         <v>7.2746090539204727E-3</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D155">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E155">
+        <v>79.85580667351411</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>15.4</v>
       </c>
@@ -2124,8 +3062,14 @@
       <c r="C156">
         <v>7.6302287457325722E-3</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D156">
+        <v>16.5</v>
+      </c>
+      <c r="E156">
+        <v>82.068156037475049</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>15.5</v>
       </c>
@@ -2135,8 +3079,14 @@
       <c r="C157">
         <v>7.7520103634242509E-3</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D157">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E157">
+        <v>97.572897467846403</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>15.6</v>
       </c>
@@ -2146,8 +3096,14 @@
       <c r="C158">
         <v>8.1226210733424727E-3</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D158">
+        <v>16.7</v>
+      </c>
+      <c r="E158">
+        <v>107.36394588029253</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>15.7</v>
       </c>
@@ -2157,8 +3113,14 @@
       <c r="C159">
         <v>8.0515109410820313E-3</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D159">
+        <v>16.8</v>
+      </c>
+      <c r="E159">
+        <v>74.133253509289887</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>15.8</v>
       </c>
@@ -2168,8 +3130,14 @@
       <c r="C160">
         <v>8.4969043746389861E-3</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D160">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E160">
+        <v>75.378543725387942</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>15.9</v>
       </c>
@@ -2179,8 +3147,14 @@
       <c r="C161">
         <v>8.6886330577831145E-3</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D161">
+        <v>17</v>
+      </c>
+      <c r="E161">
+        <v>75.091909986237113</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>16</v>
       </c>
@@ -2190,8 +3164,14 @@
       <c r="C162">
         <v>8.9895987644790024E-3</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D162">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="E162">
+        <v>75.416452945133159</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>16.100000000000001</v>
       </c>
@@ -2201,8 +3181,14 @@
       <c r="C163">
         <v>9.4031035215539818E-3</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D163">
+        <v>17.2</v>
+      </c>
+      <c r="E163">
+        <v>75.744339832437333</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>16.2</v>
       </c>
@@ -2212,8 +3198,14 @@
       <c r="C164">
         <v>9.5510597228081057E-3</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D164">
+        <v>17.3</v>
+      </c>
+      <c r="E164">
+        <v>76.186964198464182</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>16.3</v>
       </c>
@@ -2223,8 +3215,14 @@
       <c r="C165">
         <v>9.6808551504404625E-3</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D165">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E165">
+        <v>71.512623135491808</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>16.399999999999999</v>
       </c>
@@ -2234,8 +3232,14 @@
       <c r="C166">
         <v>9.8112636391351864E-3</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D166">
+        <v>17.5</v>
+      </c>
+      <c r="E166">
+        <v>73.16147296748025</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>16.5</v>
       </c>
@@ -2245,8 +3249,14 @@
       <c r="C167">
         <v>9.9387386286148537E-3</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D167">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E167">
+        <v>85.454179856820602</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>16.600000000000001</v>
       </c>
@@ -2256,8 +3266,14 @@
       <c r="C168">
         <v>9.4933805365595425E-3</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D168">
+        <v>17.7</v>
+      </c>
+      <c r="E168">
+        <v>71.09949475872763</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>16.7</v>
       </c>
@@ -2267,8 +3283,14 @@
       <c r="C169">
         <v>9.3377460270605908E-3</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D169">
+        <v>17.8</v>
+      </c>
+      <c r="E169">
+        <v>44.742276491250813</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>16.8</v>
       </c>
@@ -2278,8 +3300,14 @@
       <c r="C170">
         <v>9.3323229377589249E-3</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D170">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="E170">
+        <v>50.162252617427448</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>16.899999999999999</v>
       </c>
@@ -2289,8 +3317,14 @@
       <c r="C171">
         <v>9.1049668932793246E-3</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D171">
+        <v>18</v>
+      </c>
+      <c r="E171">
+        <v>50.434801227358328</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>17</v>
       </c>
@@ -2300,8 +3334,14 @@
       <c r="C172">
         <v>9.2152483924748535E-3</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D172">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="E172">
+        <v>50.406419214488274</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>17.100000000000001</v>
       </c>
@@ -2311,8 +3351,14 @@
       <c r="C173">
         <v>9.1231749543808725E-3</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D173">
+        <v>18.2</v>
+      </c>
+      <c r="E173">
+        <v>49.775872861444732</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>17.2</v>
       </c>
@@ -2322,8 +3368,14 @@
       <c r="C174">
         <v>8.9575767436081144E-3</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D174">
+        <v>18.3</v>
+      </c>
+      <c r="E174">
+        <v>48.89440584789088</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>17.3</v>
       </c>
@@ -2333,8 +3385,14 @@
       <c r="C175">
         <v>9.0570874247412371E-3</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D175">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="E175">
+        <v>43.830518006629603</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>17.399999999999999</v>
       </c>
@@ -2344,8 +3402,14 @@
       <c r="C176">
         <v>9.1955887379092851E-3</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D176">
+        <v>18.5</v>
+      </c>
+      <c r="E176">
+        <v>43.830518006629603</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>17.5</v>
       </c>
@@ -2355,8 +3419,14 @@
       <c r="C177">
         <v>9.3355548164795205E-3</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D177">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E177">
+        <v>40.714883761226837</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>17.600000000000001</v>
       </c>
@@ -2366,8 +3436,14 @@
       <c r="C178">
         <v>9.8697859544836439E-3</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D178">
+        <v>18.7</v>
+      </c>
+      <c r="E178">
+        <v>26.14235993076684</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>17.7</v>
       </c>
@@ -2377,8 +3453,14 @@
       <c r="C179">
         <v>1.00043953167366E-2</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D179">
+        <v>18.8</v>
+      </c>
+      <c r="E179">
+        <v>24.217483109526469</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>17.8</v>
       </c>
@@ -2388,8 +3470,14 @@
       <c r="C180">
         <v>1.0610161222934469E-2</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D180">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E180">
+        <v>29.611067087183059</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>17.899999999999999</v>
       </c>
@@ -2399,8 +3487,14 @@
       <c r="C181">
         <v>1.088535716083595E-2</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D181">
+        <v>19</v>
+      </c>
+      <c r="E181">
+        <v>28.943679586413136</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>18</v>
       </c>
@@ -2410,8 +3504,14 @@
       <c r="C182">
         <v>1.149157974840744E-2</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D182">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E182">
+        <v>26.761418550149379</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>18.100000000000001</v>
       </c>
@@ -2421,8 +3521,14 @@
       <c r="C183">
         <v>1.199873898142626E-2</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D183">
+        <v>19.2</v>
+      </c>
+      <c r="E183">
+        <v>26.052445527892029</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>18.2</v>
       </c>
@@ -2432,8 +3538,14 @@
       <c r="C184">
         <v>1.235384392629587E-2</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D184">
+        <v>19.3</v>
+      </c>
+      <c r="E184">
+        <v>25.833089508754622</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>18.3</v>
       </c>
@@ -2443,8 +3555,14 @@
       <c r="C185">
         <v>1.3010741813368641E-2</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D185">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E185">
+        <v>21.67210799299928</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>18.399999999999999</v>
       </c>
@@ -2454,8 +3572,14 @@
       <c r="C186">
         <v>1.373268393191289E-2</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D186">
+        <v>19.5</v>
+      </c>
+      <c r="E186">
+        <v>23.136371857675066</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>18.5</v>
       </c>
@@ -2465,8 +3589,14 @@
       <c r="C187">
         <v>1.4443175786515329E-2</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D187">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E187">
+        <v>28.919200618427034</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>18.600000000000001</v>
       </c>
@@ -2476,8 +3606,14 @@
       <c r="C188">
         <v>1.4868565421953009E-2</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D188">
+        <v>19.7</v>
+      </c>
+      <c r="E188">
+        <v>34.636454545190595</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>18.7</v>
       </c>
@@ -2487,8 +3623,14 @@
       <c r="C189">
         <v>1.5687280643581249E-2</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D189">
+        <v>19.8</v>
+      </c>
+      <c r="E189">
+        <v>36.56802064510304</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>18.8</v>
       </c>
@@ -2498,8 +3640,14 @@
       <c r="C190">
         <v>1.6482023323892449E-2</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D190">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E190">
+        <v>40.994696885095991</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>18.899999999999999</v>
       </c>
@@ -2509,8 +3657,14 @@
       <c r="C191">
         <v>1.681592406845607E-2</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D191">
+        <v>20</v>
+      </c>
+      <c r="E191">
+        <v>39.815066017258999</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>19</v>
       </c>
@@ -2520,8 +3674,14 @@
       <c r="C192">
         <v>1.734497005949015E-2</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D192">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E192">
+        <v>38.840961341818556</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>19.100000000000001</v>
       </c>
@@ -2531,8 +3691,14 @@
       <c r="C193">
         <v>1.7997329922285778E-2</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D193">
+        <v>20.2</v>
+      </c>
+      <c r="E193">
+        <v>38.299196915164138</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>19.2</v>
       </c>
@@ -2542,8 +3708,14 @@
       <c r="C194">
         <v>1.8195411165135851E-2</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D194">
+        <v>20.3</v>
+      </c>
+      <c r="E194">
+        <v>37.756452472243772</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>19.3</v>
       </c>
@@ -2553,8 +3725,14 @@
       <c r="C195">
         <v>1.881890100288661E-2</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D195">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E195">
+        <v>35.714769737158235</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>19.399999999999999</v>
       </c>
@@ -2564,8 +3742,14 @@
       <c r="C196">
         <v>1.9431979255617869E-2</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D196">
+        <v>20.5</v>
+      </c>
+      <c r="E196">
+        <v>38.639097961698049</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>19.5</v>
       </c>
@@ -2575,8 +3759,14 @@
       <c r="C197">
         <v>1.992177124559338E-2</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D197">
+        <v>20.6</v>
+      </c>
+      <c r="E197">
+        <v>46.967112390020596</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>19.600000000000001</v>
       </c>
@@ -2586,8 +3776,14 @@
       <c r="C198">
         <v>2.0442534454331619E-2</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D198">
+        <v>20.7</v>
+      </c>
+      <c r="E198">
+        <v>54.192718968550736</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>19.7</v>
       </c>
@@ -2597,8 +3793,14 @@
       <c r="C199">
         <v>2.0453073063481458E-2</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D199">
+        <v>20.8</v>
+      </c>
+      <c r="E199">
+        <v>52.247979865988803</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>19.8</v>
       </c>
@@ -2608,8 +3810,14 @@
       <c r="C200">
         <v>2.1092395439124941E-2</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D200">
+        <v>20.9</v>
+      </c>
+      <c r="E200">
+        <v>54.924344223103482</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>19.899999999999999</v>
       </c>
@@ -2619,8 +3827,14 @@
       <c r="C201">
         <v>2.1220334015408699E-2</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D201">
+        <v>21</v>
+      </c>
+      <c r="E201">
+        <v>54.530923602930557</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>20</v>
       </c>
@@ -2630,8 +3844,14 @@
       <c r="C202">
         <v>2.1840867983036239E-2</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D202">
+        <v>21.1</v>
+      </c>
+      <c r="E202">
+        <v>54.010195885189702</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>20.100000000000001</v>
       </c>
@@ -2641,8 +3861,14 @@
       <c r="C203">
         <v>2.2142878735066759E-2</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D203">
+        <v>21.2</v>
+      </c>
+      <c r="E203">
+        <v>53.767989160611471</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>20.2</v>
       </c>
@@ -2652,8 +3878,14 @@
       <c r="C204">
         <v>2.2699724438389669E-2</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D204">
+        <v>21.3</v>
+      </c>
+      <c r="E204">
+        <v>54.659653709242619</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>20.3</v>
       </c>
@@ -2663,8 +3895,14 @@
       <c r="C205">
         <v>2.333070799042021E-2</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D205">
+        <v>21.4</v>
+      </c>
+      <c r="E205">
+        <v>52.74865131301722</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>20.399999999999999</v>
       </c>
@@ -2674,8 +3912,14 @@
       <c r="C206">
         <v>2.3615909799571969E-2</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D206">
+        <v>21.5</v>
+      </c>
+      <c r="E206">
+        <v>55.571004346637707</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>20.5</v>
       </c>
@@ -2685,8 +3929,14 @@
       <c r="C207">
         <v>2.433576131281601E-2</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D207">
+        <v>21.6</v>
+      </c>
+      <c r="E207">
+        <v>60.127827914354725</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>20.6</v>
       </c>
@@ -2696,8 +3946,14 @@
       <c r="C208">
         <v>2.4474160744422241E-2</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D208">
+        <v>21.7</v>
+      </c>
+      <c r="E208">
+        <v>57.588458190589975</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>20.7</v>
       </c>
@@ -2707,8 +3963,14 @@
       <c r="C209">
         <v>2.3872669599431979E-2</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D209">
+        <v>21.8</v>
+      </c>
+      <c r="E209">
+        <v>49.622536012507538</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>20.8</v>
       </c>
@@ -2718,8 +3980,14 @@
       <c r="C210">
         <v>2.430020457207966E-2</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D210">
+        <v>21.9</v>
+      </c>
+      <c r="E210">
+        <v>45.850021188305909</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>20.9</v>
       </c>
@@ -2729,8 +3997,14 @@
       <c r="C211">
         <v>2.502868274065213E-2</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D211">
+        <v>22</v>
+      </c>
+      <c r="E211">
+        <v>41.242090731278786</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>21</v>
       </c>
@@ -2740,8 +4014,14 @@
       <c r="C212">
         <v>2.571590584670054E-2</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D212">
+        <v>22.1</v>
+      </c>
+      <c r="E212">
+        <v>38.747696284589011</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>21.1</v>
       </c>
@@ -2751,8 +4031,14 @@
       <c r="C213">
         <v>2.6427010434337199E-2</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D213">
+        <v>22.2</v>
+      </c>
+      <c r="E213">
+        <v>37.698221215426081</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>21.2</v>
       </c>
@@ -2762,8 +4048,14 @@
       <c r="C214">
         <v>2.7164426095724239E-2</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D214">
+        <v>22.3</v>
+      </c>
+      <c r="E214">
+        <v>37.477568206116786</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>21.3</v>
       </c>
@@ -2773,8 +4065,14 @@
       <c r="C215">
         <v>2.8158183215137449E-2</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D215">
+        <v>22.4</v>
+      </c>
+      <c r="E215">
+        <v>36.59485292714178</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>21.4</v>
       </c>
@@ -2784,8 +4082,14 @@
       <c r="C216">
         <v>2.910869962355369E-2</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D216">
+        <v>22.5</v>
+      </c>
+      <c r="E216">
+        <v>38.852185024413124</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>21.5</v>
       </c>
@@ -2795,8 +4099,14 @@
       <c r="C217">
         <v>2.9795444020981918E-2</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D217">
+        <v>22.6</v>
+      </c>
+      <c r="E217">
+        <v>40.633608236931785</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>21.6</v>
       </c>
@@ -2806,8 +4116,14 @@
       <c r="C218">
         <v>3.0228185840321529E-2</v>
       </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D218">
+        <v>22.7</v>
+      </c>
+      <c r="E218">
+        <v>35.018215002009839</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>21.7</v>
       </c>
@@ -2817,8 +4133,14 @@
       <c r="C219">
         <v>2.999453332486169E-2</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D219">
+        <v>22.8</v>
+      </c>
+      <c r="E219">
+        <v>27.765306432776253</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>21.8</v>
       </c>
@@ -2828,8 +4150,14 @@
       <c r="C220">
         <v>3.0658095919356861E-2</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D220">
+        <v>22.9</v>
+      </c>
+      <c r="E220">
+        <v>27.106239704475705</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>21.9</v>
       </c>
@@ -2839,8 +4167,14 @@
       <c r="C221">
         <v>3.1829429421893152E-2</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D221">
+        <v>23</v>
+      </c>
+      <c r="E221">
+        <v>31.732078040992203</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>22</v>
       </c>
@@ -2850,8 +4184,14 @@
       <c r="C222">
         <v>3.4140697101972137E-2</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D222">
+        <v>23.1</v>
+      </c>
+      <c r="E222">
+        <v>35.997359467669895</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>22.1</v>
       </c>
@@ -2861,8 +4201,14 @@
       <c r="C223">
         <v>3.5524488552135983E-2</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D223">
+        <v>23.2</v>
+      </c>
+      <c r="E223">
+        <v>38.539374691557924</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>22.2</v>
       </c>
@@ -2872,8 +4218,14 @@
       <c r="C224">
         <v>3.6637526596844203E-2</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D224">
+        <v>23.3</v>
+      </c>
+      <c r="E224">
+        <v>39.817697377411776</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>22.3</v>
       </c>
@@ -2883,8 +4235,14 @@
       <c r="C225">
         <v>3.7263702737356602E-2</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D225">
+        <v>23.4</v>
+      </c>
+      <c r="E225">
+        <v>38.834959259463965</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>22.4</v>
       </c>
@@ -2894,8 +4252,14 @@
       <c r="C226">
         <v>3.7798380379557427E-2</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D226">
+        <v>23.5</v>
+      </c>
+      <c r="E226">
+        <v>42.787186320021753</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>22.5</v>
       </c>
@@ -2905,8 +4269,14 @@
       <c r="C227">
         <v>3.8200292516264257E-2</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D227">
+        <v>23.6</v>
+      </c>
+      <c r="E227">
+        <v>48.800541147397304</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>22.6</v>
       </c>
@@ -2916,8 +4286,14 @@
       <c r="C228">
         <v>3.7008170245475272E-2</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D228">
+        <v>23.7</v>
+      </c>
+      <c r="E228">
+        <v>51.922242460778534</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>22.7</v>
       </c>
@@ -2927,8 +4303,14 @@
       <c r="C229">
         <v>3.7368518533452279E-2</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D229">
+        <v>23.8</v>
+      </c>
+      <c r="E229">
+        <v>59.027336228925947</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>22.8</v>
       </c>
@@ -2938,8 +4320,14 @@
       <c r="C230">
         <v>3.8396994118489389E-2</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D230">
+        <v>23.9</v>
+      </c>
+      <c r="E230">
+        <v>65.492182867862397</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>22.9</v>
       </c>
@@ -2949,8 +4337,14 @@
       <c r="C231">
         <v>3.8288899868713408E-2</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D231">
+        <v>24</v>
+      </c>
+      <c r="E231">
+        <v>67.572853209063211</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>23</v>
       </c>
@@ -2960,8 +4354,14 @@
       <c r="C232">
         <v>3.772483172761773E-2</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D232">
+        <v>24.1</v>
+      </c>
+      <c r="E232">
+        <v>69.313409483635098</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>23.1</v>
       </c>
@@ -2971,8 +4371,14 @@
       <c r="C233">
         <v>3.7245973521103599E-2</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D233">
+        <v>24.2</v>
+      </c>
+      <c r="E233">
+        <v>71.451529779715571</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>23.2</v>
       </c>
@@ -2982,8 +4388,14 @@
       <c r="C234">
         <v>3.6685991873996182E-2</v>
       </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D234">
+        <v>24.3</v>
+      </c>
+      <c r="E234">
+        <v>73.812073064560366</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>23.3</v>
       </c>
@@ -2993,8 +4405,14 @@
       <c r="C235">
         <v>3.5984103830795117E-2</v>
       </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D235">
+        <v>24.4</v>
+      </c>
+      <c r="E235">
+        <v>76.842913135769692</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>23.4</v>
       </c>
@@ -3004,8 +4422,14 @@
       <c r="C236">
         <v>3.5462625563169273E-2</v>
       </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D236">
+        <v>24.5</v>
+      </c>
+      <c r="E236">
+        <v>83.786641053180489</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>23.5</v>
       </c>
@@ -3015,8 +4439,14 @@
       <c r="C237">
         <v>3.4790302373299893E-2</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D237">
+        <v>24.6</v>
+      </c>
+      <c r="E237">
+        <v>86.89551734252133</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>23.6</v>
       </c>
@@ -3026,8 +4456,14 @@
       <c r="C238">
         <v>3.2433252980364993E-2</v>
       </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D238">
+        <v>24.7</v>
+      </c>
+      <c r="E238">
+        <v>86.187267130979492</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>23.7</v>
       </c>
@@ -3037,8 +4473,14 @@
       <c r="C239">
         <v>3.038312796999321E-2</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D239">
+        <v>24.8</v>
+      </c>
+      <c r="E239">
+        <v>83.664665596335439</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>23.8</v>
       </c>
@@ -3048,8 +4490,14 @@
       <c r="C240">
         <v>2.8345371479740492E-2</v>
       </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D240">
+        <v>24.9</v>
+      </c>
+      <c r="E240">
+        <v>80.627087139763674</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>23.9</v>
       </c>
@@ -3059,8 +4507,14 @@
       <c r="C241">
         <v>2.7323588154987598E-2</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D241">
+        <v>25</v>
+      </c>
+      <c r="E241">
+        <v>80.09863981003879</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>24</v>
       </c>
@@ -3071,7 +4525,7 @@
         <v>2.680167245975492E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>24.1</v>
       </c>
@@ -3082,7 +4536,7 @@
         <v>2.6043842199607731E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>24.2</v>
       </c>
@@ -3093,7 +4547,7 @@
         <v>2.5427017880527071E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>24.3</v>
       </c>
@@ -3104,7 +4558,7 @@
         <v>2.503648375140774E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>24.4</v>
       </c>
@@ -3115,7 +4569,7 @@
         <v>2.4279144879683551E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>24.5</v>
       </c>
@@ -3126,7 +4580,7 @@
         <v>2.3267498120673521E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>24.6</v>
       </c>
@@ -3137,7 +4591,7 @@
         <v>2.227970858789741E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>24.7</v>
       </c>
@@ -3148,7 +4602,7 @@
         <v>2.1242659023816359E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>24.8</v>
       </c>
@@ -3159,7 +4613,7 @@
         <v>2.0473676037175141E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>24.9</v>
       </c>
@@ -3170,7 +4624,7 @@
         <v>1.971590617715856E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Revert "Merge branch 'algae' of https://github.com/QSD-Group/EXPOsan into algae"
This reverts commit d645ad4f9b7fb8e224dfbc7bc81144c3aae2fb87, reversing
changes made to 9015bc346190f31b313970c59247d0248f63e300.
</commit_message>
<xml_diff>
--- a/exposan/pm2_ecorecover/data/dynamic_simul_result_calibration.xlsx
+++ b/exposan/pm2_ecorecover/data/dynamic_simul_result_calibration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Downloads\EXPOsan\exposan\pm2_ecorecover\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985C642C-754F-4E63-B05B-204235C2E47C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{904F1481-6EDE-48E0-91AF-6FDF1488E6C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{DEEFF93F-8712-407E-800A-077FF6958EEC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>t_stamp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,14 +36,6 @@
   </si>
   <si>
     <t>SP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yield_1d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>t_stamp_yield</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -409,15 +401,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47DDD832-617E-423B-B3BC-9FD3F4E9EB72}">
-  <dimension ref="A1:E252"/>
+  <dimension ref="A1:C252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D241"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,14 +419,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -444,14 +430,8 @@
       <c r="C2" s="1">
         <v>0.35744153755741681</v>
       </c>
-      <c r="D2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E2">
-        <v>141.22641287052892</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -461,14 +441,8 @@
       <c r="C3" s="1">
         <v>1.107531976471491E-2</v>
       </c>
-      <c r="D3">
-        <v>1.2</v>
-      </c>
-      <c r="E3">
-        <v>135.97279294533516</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -478,14 +452,8 @@
       <c r="C4" s="1">
         <v>8.023750326828151E-3</v>
       </c>
-      <c r="D4">
-        <v>1.3</v>
-      </c>
-      <c r="E4">
-        <v>137.25611599582237</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.3</v>
       </c>
@@ -495,14 +463,8 @@
       <c r="C5" s="1">
         <v>8.3368790863734953E-3</v>
       </c>
-      <c r="D5">
-        <v>1.4</v>
-      </c>
-      <c r="E5">
-        <v>141.4937078208886</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.4</v>
       </c>
@@ -512,14 +474,8 @@
       <c r="C6" s="1">
         <v>8.4525318869409678E-3</v>
       </c>
-      <c r="D6">
-        <v>1.5</v>
-      </c>
-      <c r="E6">
-        <v>146.22981559997456</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -529,14 +485,8 @@
       <c r="C7" s="1">
         <v>8.2427629558514404E-3</v>
       </c>
-      <c r="D7">
-        <v>1.6</v>
-      </c>
-      <c r="E7">
-        <v>155.19516202553595</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.60000000000000009</v>
       </c>
@@ -546,14 +496,8 @@
       <c r="C8" s="1">
         <v>8.047608090998748E-3</v>
       </c>
-      <c r="D8">
-        <v>1.7</v>
-      </c>
-      <c r="E8">
-        <v>164.48641289040361</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.70000000000000007</v>
       </c>
@@ -563,14 +507,8 @@
       <c r="C9" s="1">
         <v>7.6928155733528526E-3</v>
       </c>
-      <c r="D9">
-        <v>1.8</v>
-      </c>
-      <c r="E9">
-        <v>162.94445964495671</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.8</v>
       </c>
@@ -580,14 +518,8 @@
       <c r="C10" s="1">
         <v>7.5928288121893429E-3</v>
       </c>
-      <c r="D10">
-        <v>1.9</v>
-      </c>
-      <c r="E10">
-        <v>166.38433793495579</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.9</v>
       </c>
@@ -597,14 +529,8 @@
       <c r="C11" s="1">
         <v>7.7011487317907162E-3</v>
       </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>171.90915255790085</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -614,14 +540,8 @@
       <c r="C12" s="1">
         <v>7.7124903485505016E-3</v>
       </c>
-      <c r="D12">
-        <v>2.1</v>
-      </c>
-      <c r="E12">
-        <v>185.10118651133465</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1.1000000000000001</v>
       </c>
@@ -631,14 +551,8 @@
       <c r="C13" s="1">
         <v>7.6850542823217946E-3</v>
       </c>
-      <c r="D13">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E13">
-        <v>194.07285149384563</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1.2</v>
       </c>
@@ -648,14 +562,8 @@
       <c r="C14" s="1">
         <v>7.5907843687077828E-3</v>
       </c>
-      <c r="D14">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E14">
-        <v>204.71501041834455</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1.3</v>
       </c>
@@ -665,14 +573,8 @@
       <c r="C15" s="1">
         <v>7.4713145778358223E-3</v>
       </c>
-      <c r="D15">
-        <v>2.4</v>
-      </c>
-      <c r="E15">
-        <v>218.07116024736308</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1.4</v>
       </c>
@@ -682,14 +584,8 @@
       <c r="C16" s="1">
         <v>7.4172540833685281E-3</v>
       </c>
-      <c r="D16">
-        <v>2.5</v>
-      </c>
-      <c r="E16">
-        <v>238.31941931582114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1.5</v>
       </c>
@@ -699,14 +595,8 @@
       <c r="C17" s="1">
         <v>7.1545651875343577E-3</v>
       </c>
-      <c r="D17">
-        <v>2.6</v>
-      </c>
-      <c r="E17">
-        <v>272.09624752272452</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1.6</v>
       </c>
@@ -716,14 +606,8 @@
       <c r="C18" s="1">
         <v>6.8176199738561108E-3</v>
       </c>
-      <c r="D18">
-        <v>2.7</v>
-      </c>
-      <c r="E18">
-        <v>307.41925825383117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1.7</v>
       </c>
@@ -733,14 +617,8 @@
       <c r="C19" s="1">
         <v>6.4030155962494471E-3</v>
       </c>
-      <c r="D19">
-        <v>2.8</v>
-      </c>
-      <c r="E19">
-        <v>311.20108197779354</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1.8</v>
       </c>
@@ -750,14 +628,8 @@
       <c r="C20" s="1">
         <v>6.1844623865160526E-3</v>
       </c>
-      <c r="D20">
-        <v>2.9</v>
-      </c>
-      <c r="E20">
-        <v>316.16888749769345</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1.9</v>
       </c>
@@ -767,14 +639,8 @@
       <c r="C21" s="1">
         <v>5.890199985453818E-3</v>
       </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
-      <c r="E21">
-        <v>326.15154922902803</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -784,14 +650,8 @@
       <c r="C22" s="1">
         <v>5.6469543849011847E-3</v>
       </c>
-      <c r="D22">
-        <v>3.1</v>
-      </c>
-      <c r="E22">
-        <v>324.02324436213377</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2.1</v>
       </c>
@@ -801,14 +661,8 @@
       <c r="C23" s="1">
         <v>5.3266579662909798E-3</v>
       </c>
-      <c r="D23">
-        <v>3.2</v>
-      </c>
-      <c r="E23">
-        <v>315.57106974593427</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2.2000000000000002</v>
       </c>
@@ -818,14 +672,8 @@
       <c r="C24" s="1">
         <v>4.9245021171890301E-3</v>
       </c>
-      <c r="D24">
-        <v>3.3</v>
-      </c>
-      <c r="E24">
-        <v>305.0056768948071</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2.2999999999999998</v>
       </c>
@@ -835,14 +683,8 @@
       <c r="C25" s="1">
         <v>4.4682823813590924E-3</v>
       </c>
-      <c r="D25">
-        <v>3.4</v>
-      </c>
-      <c r="E25">
-        <v>296.98411351130693</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2.4</v>
       </c>
@@ -852,14 +694,8 @@
       <c r="C26" s="1">
         <v>4.1120777190817859E-3</v>
       </c>
-      <c r="D26">
-        <v>3.5</v>
-      </c>
-      <c r="E26">
-        <v>290.32990663325063</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2.5</v>
       </c>
@@ -869,14 +705,8 @@
       <c r="C27" s="1">
         <v>3.900444179544525E-3</v>
       </c>
-      <c r="D27">
-        <v>3.6</v>
-      </c>
-      <c r="E27">
-        <v>281.10983535961992</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2.6</v>
       </c>
@@ -886,14 +716,8 @@
       <c r="C28" s="1">
         <v>3.662563688739968E-3</v>
       </c>
-      <c r="D28">
-        <v>3.7</v>
-      </c>
-      <c r="E28">
-        <v>263.79042643133266</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2.7</v>
       </c>
@@ -903,14 +727,8 @@
       <c r="C29" s="1">
         <v>3.5054778851214912E-3</v>
       </c>
-      <c r="D29">
-        <v>3.8</v>
-      </c>
-      <c r="E29">
-        <v>217.35976430814989</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2.8</v>
       </c>
@@ -920,14 +738,8 @@
       <c r="C30" s="1">
         <v>3.4563613546098049E-3</v>
       </c>
-      <c r="D30">
-        <v>3.9</v>
-      </c>
-      <c r="E30">
-        <v>185.49583065482707</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2.9</v>
       </c>
@@ -937,14 +749,8 @@
       <c r="C31" s="1">
         <v>3.5341997975597739E-3</v>
       </c>
-      <c r="D31">
-        <v>4</v>
-      </c>
-      <c r="E31">
-        <v>164.67647430927929</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -954,14 +760,8 @@
       <c r="C32" s="1">
         <v>3.6180510852257151E-3</v>
       </c>
-      <c r="D32">
-        <v>4.1000000000000014</v>
-      </c>
-      <c r="E32">
-        <v>143.97381475632523</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3.1</v>
       </c>
@@ -971,14 +771,8 @@
       <c r="C33" s="1">
         <v>3.963679945281906E-3</v>
       </c>
-      <c r="D33">
-        <v>4.2</v>
-      </c>
-      <c r="E33">
-        <v>133.95044793283728</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3.2</v>
       </c>
@@ -988,14 +782,8 @@
       <c r="C34" s="1">
         <v>4.1607249923814628E-3</v>
       </c>
-      <c r="D34">
-        <v>4.3</v>
-      </c>
-      <c r="E34">
-        <v>128.69920570803458</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3.3</v>
       </c>
@@ -1005,14 +793,8 @@
       <c r="C35" s="1">
         <v>4.4811730158857681E-3</v>
       </c>
-      <c r="D35">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E35">
-        <v>125.82675414951444</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>3.4</v>
       </c>
@@ -1022,14 +804,8 @@
       <c r="C36" s="1">
         <v>4.9060457617201708E-3</v>
       </c>
-      <c r="D36">
-        <v>4.5</v>
-      </c>
-      <c r="E36">
-        <v>122.31902451577163</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>3.5</v>
       </c>
@@ -1039,14 +815,8 @@
       <c r="C37" s="1">
         <v>5.375602114115423E-3</v>
       </c>
-      <c r="D37">
-        <v>4.6000000000000014</v>
-      </c>
-      <c r="E37">
-        <v>119.08849859686953</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>3.6</v>
       </c>
@@ -1056,14 +826,8 @@
       <c r="C38" s="1">
         <v>5.7965711613269539E-3</v>
       </c>
-      <c r="D38">
-        <v>4.7</v>
-      </c>
-      <c r="E38">
-        <v>107.75993290630599</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3.7</v>
       </c>
@@ -1073,14 +837,8 @@
       <c r="C39" s="1">
         <v>6.1668751874600428E-3</v>
       </c>
-      <c r="D39">
-        <v>4.8000000000000007</v>
-      </c>
-      <c r="E39">
-        <v>80.454469551759615</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>3.8</v>
       </c>
@@ -1090,14 +848,8 @@
       <c r="C40" s="1">
         <v>6.7841741523916137E-3</v>
       </c>
-      <c r="D40">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E40">
-        <v>70.6610342144795</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>3.9</v>
       </c>
@@ -1107,14 +859,8 @@
       <c r="C41" s="1">
         <v>7.3934642554173398E-3</v>
       </c>
-      <c r="D41">
-        <v>5</v>
-      </c>
-      <c r="E41">
-        <v>69.105060705339895</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1124,14 +870,8 @@
       <c r="C42" s="1">
         <v>8.0319126961436119E-3</v>
       </c>
-      <c r="D42">
-        <v>5.1000000000000014</v>
-      </c>
-      <c r="E42">
-        <v>67.769369182296799</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4.1000000000000014</v>
       </c>
@@ -1141,14 +881,8 @@
       <c r="C43" s="1">
         <v>8.7566441485514932E-3</v>
       </c>
-      <c r="D43">
-        <v>5.2</v>
-      </c>
-      <c r="E43">
-        <v>66.622472229871377</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>4.2</v>
       </c>
@@ -1158,14 +892,8 @@
       <c r="C44" s="1">
         <v>9.340020468893314E-3</v>
       </c>
-      <c r="D44">
-        <v>5.3000000000000007</v>
-      </c>
-      <c r="E44">
-        <v>65.734720727098164</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>4.3</v>
       </c>
@@ -1175,14 +903,8 @@
       <c r="C45" s="1">
         <v>1.005687504009666E-2</v>
       </c>
-      <c r="D45">
-        <v>5.4</v>
-      </c>
-      <c r="E45">
-        <v>66.91647524561543</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>4.4000000000000004</v>
       </c>
@@ -1192,14 +914,8 @@
       <c r="C46" s="1">
         <v>1.056710418044126E-2</v>
       </c>
-      <c r="D46">
-        <v>5.5</v>
-      </c>
-      <c r="E46">
-        <v>69.792775866637314</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4.5</v>
       </c>
@@ -1209,14 +925,8 @@
       <c r="C47" s="1">
         <v>1.1050850441609439E-2</v>
       </c>
-      <c r="D47">
-        <v>5.6000000000000014</v>
-      </c>
-      <c r="E47">
-        <v>71.999558753876386</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>4.6000000000000014</v>
       </c>
@@ -1226,14 +936,8 @@
       <c r="C48" s="1">
         <v>1.1393393895568831E-2</v>
       </c>
-      <c r="D48">
-        <v>5.7</v>
-      </c>
-      <c r="E48">
-        <v>69.889997832841473</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4.7</v>
       </c>
@@ -1243,14 +947,8 @@
       <c r="C49" s="1">
         <v>1.166064289197348E-2</v>
       </c>
-      <c r="D49">
-        <v>5.8000000000000007</v>
-      </c>
-      <c r="E49">
-        <v>62.205462418638056</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>4.8000000000000007</v>
       </c>
@@ -1260,14 +958,8 @@
       <c r="C50" s="1">
         <v>1.199332966342577E-2</v>
       </c>
-      <c r="D50">
-        <v>5.9</v>
-      </c>
-      <c r="E50">
-        <v>58.996395382408672</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>4.9000000000000004</v>
       </c>
@@ -1277,14 +969,8 @@
       <c r="C51" s="1">
         <v>1.226872553654202E-2</v>
       </c>
-      <c r="D51">
-        <v>6</v>
-      </c>
-      <c r="E51">
-        <v>59.091189459017215</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>5</v>
       </c>
@@ -1294,14 +980,8 @@
       <c r="C52" s="1">
         <v>1.2707943516759209E-2</v>
       </c>
-      <c r="D52">
-        <v>6.1000000000000014</v>
-      </c>
-      <c r="E52">
-        <v>59.297671256470601</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5.1000000000000014</v>
       </c>
@@ -1311,14 +991,8 @@
       <c r="C53" s="1">
         <v>1.3117618006091E-2</v>
       </c>
-      <c r="D53">
-        <v>6.2</v>
-      </c>
-      <c r="E53">
-        <v>59.666896195248796</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>5.2</v>
       </c>
@@ -1328,14 +1002,8 @@
       <c r="C54" s="1">
         <v>1.324983839921591E-2</v>
       </c>
-      <c r="D54">
-        <v>6.3000000000000007</v>
-      </c>
-      <c r="E54">
-        <v>60.169494063175463</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>5.3000000000000007</v>
       </c>
@@ -1345,14 +1013,8 @@
       <c r="C55" s="1">
         <v>1.364164342781549E-2</v>
       </c>
-      <c r="D55">
-        <v>6.4</v>
-      </c>
-      <c r="E55">
-        <v>62.273426130964296</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>5.4</v>
       </c>
@@ -1362,14 +1024,8 @@
       <c r="C56" s="1">
         <v>1.369136083747537E-2</v>
       </c>
-      <c r="D56">
-        <v>6.5</v>
-      </c>
-      <c r="E56">
-        <v>64.850657243796263</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>5.5</v>
       </c>
@@ -1379,14 +1035,8 @@
       <c r="C57" s="1">
         <v>1.391303899136772E-2</v>
       </c>
-      <c r="D57">
-        <v>6.6000000000000014</v>
-      </c>
-      <c r="E57">
-        <v>66.648301432291248</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>5.6000000000000014</v>
       </c>
@@ -1396,14 +1046,8 @@
       <c r="C58" s="1">
         <v>1.3763069438431389E-2</v>
       </c>
-      <c r="D58">
-        <v>6.7</v>
-      </c>
-      <c r="E58">
-        <v>66.326706835516902</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>5.7</v>
       </c>
@@ -1413,14 +1057,8 @@
       <c r="C59" s="1">
         <v>1.387122135430891E-2</v>
       </c>
-      <c r="D59">
-        <v>6.8000000000000007</v>
-      </c>
-      <c r="E59">
-        <v>61.901482579563634</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>5.8000000000000007</v>
       </c>
@@ -1430,14 +1068,8 @@
       <c r="C60" s="1">
         <v>1.385835732877426E-2</v>
       </c>
-      <c r="D60">
-        <v>6.9</v>
-      </c>
-      <c r="E60">
-        <v>60.457148802318507</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>5.9</v>
       </c>
@@ -1447,14 +1079,8 @@
       <c r="C61" s="1">
         <v>1.4215790718244491E-2</v>
       </c>
-      <c r="D61">
-        <v>7</v>
-      </c>
-      <c r="E61">
-        <v>62.838532845573553</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>6</v>
       </c>
@@ -1464,14 +1090,8 @@
       <c r="C62" s="1">
         <v>1.4306328030382891E-2</v>
       </c>
-      <c r="D62">
-        <v>7.1000000000000014</v>
-      </c>
-      <c r="E62">
-        <v>66.161927305941902</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>6.1000000000000014</v>
       </c>
@@ -1481,14 +1101,8 @@
       <c r="C63" s="1">
         <v>1.465699042511567E-2</v>
       </c>
-      <c r="D63">
-        <v>7.2</v>
-      </c>
-      <c r="E63">
-        <v>69.524153233279534</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>6.2</v>
       </c>
@@ -1498,14 +1112,8 @@
       <c r="C64" s="1">
         <v>1.4793210369891259E-2</v>
       </c>
-      <c r="D64">
-        <v>7.3000000000000007</v>
-      </c>
-      <c r="E64">
-        <v>72.138253257486539</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>6.3000000000000007</v>
       </c>
@@ -1515,14 +1123,8 @@
       <c r="C65" s="1">
         <v>1.503102911195551E-2</v>
       </c>
-      <c r="D65">
-        <v>7.4</v>
-      </c>
-      <c r="E65">
-        <v>75.030372357463406</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>6.4</v>
       </c>
@@ -1532,14 +1134,8 @@
       <c r="C66" s="1">
         <v>1.5295859825186719E-2</v>
       </c>
-      <c r="D66">
-        <v>7.5</v>
-      </c>
-      <c r="E66">
-        <v>78.366202266904381</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>6.5</v>
       </c>
@@ -1549,14 +1145,8 @@
       <c r="C67" s="1">
         <v>1.527187094526922E-2</v>
       </c>
-      <c r="D67">
-        <v>7.6000000000000014</v>
-      </c>
-      <c r="E67">
-        <v>80.690828485220308</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>6.6000000000000014</v>
       </c>
@@ -1566,14 +1156,8 @@
       <c r="C68" s="1">
         <v>1.5306904098264389E-2</v>
       </c>
-      <c r="D68">
-        <v>7.7</v>
-      </c>
-      <c r="E68">
-        <v>84.527857271848703</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>6.7</v>
       </c>
@@ -1583,14 +1167,8 @@
       <c r="C69" s="1">
         <v>1.5299679827600981E-2</v>
       </c>
-      <c r="D69">
-        <v>7.8000000000000007</v>
-      </c>
-      <c r="E69">
-        <v>79.56130898264756</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>6.8000000000000007</v>
       </c>
@@ -1600,14 +1178,8 @@
       <c r="C70" s="1">
         <v>1.5198612509803521E-2</v>
       </c>
-      <c r="D70">
-        <v>7.9</v>
-      </c>
-      <c r="E70">
-        <v>71.996111088716148</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>6.9</v>
       </c>
@@ -1617,14 +1189,8 @@
       <c r="C71" s="1">
         <v>1.528280404432324E-2</v>
       </c>
-      <c r="D71">
-        <v>8</v>
-      </c>
-      <c r="E71">
-        <v>67.896267524560074</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>7</v>
       </c>
@@ -1634,14 +1200,8 @@
       <c r="C72" s="1">
         <v>1.5302512144562141E-2</v>
       </c>
-      <c r="D72">
-        <v>8.1</v>
-      </c>
-      <c r="E72">
-        <v>66.181918062494347</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>7.1000000000000014</v>
       </c>
@@ -1651,14 +1211,8 @@
       <c r="C73" s="1">
         <v>1.5202374297606919E-2</v>
       </c>
-      <c r="D73">
-        <v>8.2000000000000011</v>
-      </c>
-      <c r="E73">
-        <v>64.035443585099245</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>7.2</v>
       </c>
@@ -1668,14 +1222,8 @@
       <c r="C74" s="1">
         <v>1.5050079679233139E-2</v>
       </c>
-      <c r="D74">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="E74">
-        <v>62.062452959333221</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>7.3000000000000007</v>
       </c>
@@ -1685,14 +1233,8 @@
       <c r="C75" s="1">
         <v>1.521206802512476E-2</v>
       </c>
-      <c r="D75">
-        <v>8.4</v>
-      </c>
-      <c r="E75">
-        <v>62.509860016672995</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>7.4</v>
       </c>
@@ -1702,14 +1244,8 @@
       <c r="C76" s="1">
         <v>1.554036744227931E-2</v>
       </c>
-      <c r="D76">
-        <v>8.5</v>
-      </c>
-      <c r="E76">
-        <v>64.361445104550242</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>7.5</v>
       </c>
@@ -1719,14 +1255,8 @@
       <c r="C77" s="1">
         <v>1.557397797271105E-2</v>
       </c>
-      <c r="D77">
-        <v>8.6</v>
-      </c>
-      <c r="E77">
-        <v>67.97017108583151</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>7.6000000000000014</v>
       </c>
@@ -1736,14 +1266,8 @@
       <c r="C78" s="1">
         <v>1.579028696060486E-2</v>
       </c>
-      <c r="D78">
-        <v>8.7000000000000011</v>
-      </c>
-      <c r="E78">
-        <v>73.756488747295904</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>7.7</v>
       </c>
@@ -1753,14 +1277,8 @@
       <c r="C79" s="1">
         <v>1.544228227985996E-2</v>
       </c>
-      <c r="D79">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="E79">
-        <v>69.104290423400585</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>7.8000000000000007</v>
       </c>
@@ -1770,14 +1288,8 @@
       <c r="C80" s="1">
         <v>1.5649686977813351E-2</v>
       </c>
-      <c r="D80">
-        <v>8.9</v>
-      </c>
-      <c r="E80">
-        <v>67.356434819572897</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>7.9</v>
       </c>
@@ -1787,14 +1299,8 @@
       <c r="C81" s="1">
         <v>1.5980002786042509E-2</v>
       </c>
-      <c r="D81">
-        <v>9</v>
-      </c>
-      <c r="E81">
-        <v>72.006876520816348</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>8</v>
       </c>
@@ -1804,14 +1310,8 @@
       <c r="C82" s="1">
         <v>1.6729880685912229E-2</v>
       </c>
-      <c r="D82">
-        <v>9.1</v>
-      </c>
-      <c r="E82">
-        <v>76.912306483218003</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>8.1</v>
       </c>
@@ -1821,14 +1321,8 @@
       <c r="C83" s="1">
         <v>1.6759911977767449E-2</v>
       </c>
-      <c r="D83">
-        <v>9.2000000000000011</v>
-      </c>
-      <c r="E83">
-        <v>78.595175802044309</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>8.2000000000000011</v>
       </c>
@@ -1838,14 +1332,8 @@
       <c r="C84" s="1">
         <v>1.67846543111933E-2</v>
       </c>
-      <c r="D84">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="E84">
-        <v>80.106090167518261</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>8.3000000000000007</v>
       </c>
@@ -1855,14 +1343,8 @@
       <c r="C85" s="1">
         <v>1.6594358724505359E-2</v>
       </c>
-      <c r="D85">
-        <v>9.4</v>
-      </c>
-      <c r="E85">
-        <v>83.524617936634399</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>8.4</v>
       </c>
@@ -1872,14 +1354,8 @@
       <c r="C86" s="1">
         <v>1.6344963736168679E-2</v>
       </c>
-      <c r="D86">
-        <v>9.5</v>
-      </c>
-      <c r="E86">
-        <v>88.966936865417466</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>8.5</v>
       </c>
@@ -1889,14 +1365,8 @@
       <c r="C87" s="1">
         <v>1.6002392676923591E-2</v>
       </c>
-      <c r="D87">
-        <v>9.6000000000000014</v>
-      </c>
-      <c r="E87">
-        <v>93.385143939669902</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>8.6</v>
       </c>
@@ -1906,14 +1376,8 @@
       <c r="C88" s="1">
         <v>1.552642384107283E-2</v>
       </c>
-      <c r="D88">
-        <v>9.7000000000000011</v>
-      </c>
-      <c r="E88">
-        <v>97.714759568979829</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>8.7000000000000011</v>
       </c>
@@ -1923,14 +1387,8 @@
       <c r="C89" s="1">
         <v>1.457597872810504E-2</v>
       </c>
-      <c r="D89">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="E89">
-        <v>89.837050977472032</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>8.8000000000000007</v>
       </c>
@@ -1940,14 +1398,8 @@
       <c r="C90" s="1">
         <v>1.4167911938584561E-2</v>
       </c>
-      <c r="D90">
-        <v>9.9</v>
-      </c>
-      <c r="E90">
-        <v>84.685777993895087</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>8.9</v>
       </c>
@@ -1957,14 +1409,8 @@
       <c r="C91" s="1">
         <v>1.39619055632788E-2</v>
       </c>
-      <c r="D91">
-        <v>10</v>
-      </c>
-      <c r="E91">
-        <v>84.276444503853838</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>9</v>
       </c>
@@ -1974,14 +1420,8 @@
       <c r="C92" s="1">
         <v>1.371319055641233E-2</v>
       </c>
-      <c r="D92">
-        <v>10.1</v>
-      </c>
-      <c r="E92">
-        <v>82.39011785191704</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>9.1</v>
       </c>
@@ -1991,14 +1431,8 @@
       <c r="C93" s="1">
         <v>1.3410869000320491E-2</v>
       </c>
-      <c r="D93">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="E93">
-        <v>82.192089179606214</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>9.2000000000000011</v>
       </c>
@@ -2008,14 +1442,8 @@
       <c r="C94" s="1">
         <v>1.309901987120321E-2</v>
       </c>
-      <c r="D94">
-        <v>10.3</v>
-      </c>
-      <c r="E94">
-        <v>82.473039790810247</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>9.3000000000000007</v>
       </c>
@@ -2025,14 +1453,8 @@
       <c r="C95" s="1">
         <v>1.2785479007028099E-2</v>
       </c>
-      <c r="D95">
-        <v>10.4</v>
-      </c>
-      <c r="E95">
-        <v>83.736316238605241</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>9.4</v>
       </c>
@@ -2042,14 +1464,8 @@
       <c r="C96" s="1">
         <v>1.236175574158252E-2</v>
       </c>
-      <c r="D96">
-        <v>10.5</v>
-      </c>
-      <c r="E96">
-        <v>85.188818895842346</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>9.5</v>
       </c>
@@ -2059,14 +1475,8 @@
       <c r="C97" s="1">
         <v>1.1823278127276749E-2</v>
       </c>
-      <c r="D97">
-        <v>10.6</v>
-      </c>
-      <c r="E97">
-        <v>84.269834050745573</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>9.6000000000000014</v>
       </c>
@@ -2076,14 +1486,8 @@
       <c r="C98" s="1">
         <v>1.139245045375299E-2</v>
       </c>
-      <c r="D98">
-        <v>10.7</v>
-      </c>
-      <c r="E98">
-        <v>81.745703681267173</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>9.7000000000000011</v>
       </c>
@@ -2093,14 +1497,8 @@
       <c r="C99" s="1">
         <v>1.0919789190071199E-2</v>
       </c>
-      <c r="D99">
-        <v>10.8</v>
-      </c>
-      <c r="E99">
-        <v>73.31680498787108</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>9.8000000000000007</v>
       </c>
@@ -2110,14 +1508,8 @@
       <c r="C100" s="1">
         <v>1.0540817049596189E-2</v>
       </c>
-      <c r="D100">
-        <v>10.9</v>
-      </c>
-      <c r="E100">
-        <v>73.024892627670155</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>9.9</v>
       </c>
@@ -2127,14 +1519,8 @@
       <c r="C101" s="1">
         <v>1.025390064694965E-2</v>
       </c>
-      <c r="D101">
-        <v>11</v>
-      </c>
-      <c r="E101">
-        <v>76.171723874362442</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>10</v>
       </c>
@@ -2144,14 +1530,8 @@
       <c r="C102" s="1">
         <v>9.9826400208533686E-3</v>
       </c>
-      <c r="D102">
-        <v>11.1</v>
-      </c>
-      <c r="E102">
-        <v>79.731468800898838</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>10.1</v>
       </c>
@@ -2161,14 +1541,8 @@
       <c r="C103" s="1">
         <v>9.6883819608733143E-3</v>
       </c>
-      <c r="D103">
-        <v>11.2</v>
-      </c>
-      <c r="E103">
-        <v>84.926117407681105</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>10.199999999999999</v>
       </c>
@@ -2178,14 +1552,8 @@
       <c r="C104" s="1">
         <v>9.2910202099324244E-3</v>
       </c>
-      <c r="D104">
-        <v>11.3</v>
-      </c>
-      <c r="E104">
-        <v>88.196861862918013</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>10.3</v>
       </c>
@@ -2195,14 +1563,8 @@
       <c r="C105" s="1">
         <v>8.8389841353768046E-3</v>
       </c>
-      <c r="D105">
-        <v>11.4</v>
-      </c>
-      <c r="E105">
-        <v>93.162862203673726</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>10.4</v>
       </c>
@@ -2212,14 +1574,8 @@
       <c r="C106" s="1">
         <v>8.3701684432845314E-3</v>
       </c>
-      <c r="D106">
-        <v>11.5</v>
-      </c>
-      <c r="E106">
-        <v>103.4426825283621</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>10.5</v>
       </c>
@@ -2229,14 +1585,8 @@
       <c r="C107" s="1">
         <v>8.0773493100987238E-3</v>
       </c>
-      <c r="D107">
-        <v>11.6</v>
-      </c>
-      <c r="E107">
-        <v>109.03260580205861</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>10.6</v>
       </c>
@@ -2246,14 +1596,8 @@
       <c r="C108" s="1">
         <v>7.7857282493948247E-3</v>
       </c>
-      <c r="D108">
-        <v>11.7</v>
-      </c>
-      <c r="E108">
-        <v>113.72818004229948</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>10.7</v>
       </c>
@@ -2263,14 +1607,8 @@
       <c r="C109" s="1">
         <v>7.4779006302009791E-3</v>
       </c>
-      <c r="D109">
-        <v>11.8</v>
-      </c>
-      <c r="E109">
-        <v>115.00859453318331</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>10.8</v>
       </c>
@@ -2280,14 +1618,8 @@
       <c r="C110" s="1">
         <v>7.2986977702901128E-3</v>
       </c>
-      <c r="D110">
-        <v>11.9</v>
-      </c>
-      <c r="E110">
-        <v>114.76792465710119</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>10.9</v>
       </c>
@@ -2297,14 +1629,8 @@
       <c r="C111" s="1">
         <v>7.1549567989567789E-3</v>
       </c>
-      <c r="D111">
-        <v>12</v>
-      </c>
-      <c r="E111">
-        <v>115.17166502180503</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>11</v>
       </c>
@@ -2314,14 +1640,8 @@
       <c r="C112" s="1">
         <v>6.9610729085756969E-3</v>
       </c>
-      <c r="D112">
-        <v>12.1</v>
-      </c>
-      <c r="E112">
-        <v>116.01924680569674</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>11.1</v>
       </c>
@@ -2331,14 +1651,8 @@
       <c r="C113" s="1">
         <v>6.7900989115672744E-3</v>
       </c>
-      <c r="D113">
-        <v>12.2</v>
-      </c>
-      <c r="E113">
-        <v>116.58742112065853</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>11.2</v>
       </c>
@@ -2348,14 +1662,8 @@
       <c r="C114" s="1">
         <v>6.8278936740797597E-3</v>
       </c>
-      <c r="D114">
-        <v>12.3</v>
-      </c>
-      <c r="E114">
-        <v>117.28985356508851</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>11.3</v>
       </c>
@@ -2365,14 +1673,8 @@
       <c r="C115" s="1">
         <v>6.6296016918297312E-3</v>
       </c>
-      <c r="D115">
-        <v>12.4</v>
-      </c>
-      <c r="E115">
-        <v>121.21788906979003</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>11.4</v>
       </c>
@@ -2382,14 +1684,8 @@
       <c r="C116" s="1">
         <v>6.6811396618864224E-3</v>
       </c>
-      <c r="D116">
-        <v>12.5</v>
-      </c>
-      <c r="E116">
-        <v>130.51844692658599</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>11.5</v>
       </c>
@@ -2399,14 +1695,8 @@
       <c r="C117" s="1">
         <v>6.5243756549859134E-3</v>
       </c>
-      <c r="D117">
-        <v>12.6</v>
-      </c>
-      <c r="E117">
-        <v>135.70093781055797</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>11.6</v>
       </c>
@@ -2416,14 +1706,8 @@
       <c r="C118" s="1">
         <v>6.4405641662449113E-3</v>
       </c>
-      <c r="D118">
-        <v>12.7</v>
-      </c>
-      <c r="E118">
-        <v>143.88913505087058</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>11.7</v>
       </c>
@@ -2433,14 +1717,8 @@
       <c r="C119" s="1">
         <v>6.4784934559068523E-3</v>
       </c>
-      <c r="D119">
-        <v>12.8</v>
-      </c>
-      <c r="E119">
-        <v>145.26423136997519</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>11.8</v>
       </c>
@@ -2450,14 +1728,8 @@
       <c r="C120" s="1">
         <v>6.325693973864753E-3</v>
       </c>
-      <c r="D120">
-        <v>12.9</v>
-      </c>
-      <c r="E120">
-        <v>141.00582242427657</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>11.9</v>
       </c>
@@ -2467,14 +1739,8 @@
       <c r="C121" s="1">
         <v>6.3407840360676336E-3</v>
       </c>
-      <c r="D121">
-        <v>13</v>
-      </c>
-      <c r="E121">
-        <v>140.58004266612076</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>12</v>
       </c>
@@ -2484,14 +1750,8 @@
       <c r="C122" s="1">
         <v>6.4335562604397418E-3</v>
       </c>
-      <c r="D122">
-        <v>13.1</v>
-      </c>
-      <c r="E122">
-        <v>139.85438078728146</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>12.1</v>
       </c>
@@ -2501,14 +1761,8 @@
       <c r="C123" s="1">
         <v>6.2362993685006994E-3</v>
       </c>
-      <c r="D123">
-        <v>13.2</v>
-      </c>
-      <c r="E123">
-        <v>138.42919754476924</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>12.2</v>
       </c>
@@ -2518,14 +1772,8 @@
       <c r="C124" s="1">
         <v>6.3025833835089872E-3</v>
       </c>
-      <c r="D124">
-        <v>13.3</v>
-      </c>
-      <c r="E124">
-        <v>136.75807144930806</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>12.3</v>
       </c>
@@ -2535,14 +1783,8 @@
       <c r="C125" s="1">
         <v>6.3887410656872931E-3</v>
       </c>
-      <c r="D125">
-        <v>13.4</v>
-      </c>
-      <c r="E125">
-        <v>136.33096750496463</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>12.4</v>
       </c>
@@ -2552,14 +1794,8 @@
       <c r="C126" s="1">
         <v>6.1514519382426646E-3</v>
       </c>
-      <c r="D126">
-        <v>13.5</v>
-      </c>
-      <c r="E126">
-        <v>138.49194783720057</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>12.5</v>
       </c>
@@ -2569,14 +1805,8 @@
       <c r="C127" s="1">
         <v>6.1760566090801623E-3</v>
       </c>
-      <c r="D127">
-        <v>13.6</v>
-      </c>
-      <c r="E127">
-        <v>136.93572900130602</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>12.6</v>
       </c>
@@ -2586,14 +1816,8 @@
       <c r="C128" s="1">
         <v>5.9427329344435391E-3</v>
       </c>
-      <c r="D128">
-        <v>13.7</v>
-      </c>
-      <c r="E128">
-        <v>128.51617440954612</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>12.7</v>
       </c>
@@ -2603,14 +1827,8 @@
       <c r="C129" s="1">
         <v>5.9120398319980469E-3</v>
       </c>
-      <c r="D129">
-        <v>13.8</v>
-      </c>
-      <c r="E129">
-        <v>115.34741378531913</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>12.8</v>
       </c>
@@ -2620,14 +1838,8 @@
       <c r="C130" s="1">
         <v>5.9660813791428836E-3</v>
       </c>
-      <c r="D130">
-        <v>13.9</v>
-      </c>
-      <c r="E130">
-        <v>103.29798606292611</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>12.9</v>
       </c>
@@ -2637,14 +1849,8 @@
       <c r="C131" s="1">
         <v>6.0643245431174489E-3</v>
       </c>
-      <c r="D131">
-        <v>14</v>
-      </c>
-      <c r="E131">
-        <v>101.11411408429127</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>13</v>
       </c>
@@ -2654,14 +1860,8 @@
       <c r="C132" s="1">
         <v>6.4882603096759724E-3</v>
       </c>
-      <c r="D132">
-        <v>14.1</v>
-      </c>
-      <c r="E132">
-        <v>99.133180300042525</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>13.1</v>
       </c>
@@ -2671,14 +1871,8 @@
       <c r="C133" s="1">
         <v>6.6174701543940959E-3</v>
       </c>
-      <c r="D133">
-        <v>14.2</v>
-      </c>
-      <c r="E133">
-        <v>97.597777919000819</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>13.2</v>
       </c>
@@ -2688,14 +1882,8 @@
       <c r="C134" s="1">
         <v>7.0581802478038164E-3</v>
       </c>
-      <c r="D134">
-        <v>14.3</v>
-      </c>
-      <c r="E134">
-        <v>96.767501424670527</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>13.3</v>
       </c>
@@ -2705,14 +1893,8 @@
       <c r="C135" s="1">
         <v>7.505469630874553E-3</v>
       </c>
-      <c r="D135">
-        <v>14.4</v>
-      </c>
-      <c r="E135">
-        <v>90.590565816466537</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>13.4</v>
       </c>
@@ -2722,14 +1904,8 @@
       <c r="C136" s="1">
         <v>7.9628694494917555E-3</v>
       </c>
-      <c r="D136">
-        <v>14.5</v>
-      </c>
-      <c r="E136">
-        <v>84.297989863776309</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>13.5</v>
       </c>
@@ -2739,14 +1915,8 @@
       <c r="C137" s="1">
         <v>8.3662689757695204E-3</v>
       </c>
-      <c r="D137">
-        <v>14.6</v>
-      </c>
-      <c r="E137">
-        <v>84.029982610536905</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>13.6</v>
       </c>
@@ -2756,14 +1926,8 @@
       <c r="C138" s="1">
         <v>8.7090820048649521E-3</v>
       </c>
-      <c r="D138">
-        <v>14.7</v>
-      </c>
-      <c r="E138">
-        <v>96.256559634257712</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>13.7</v>
       </c>
@@ -2773,14 +1937,8 @@
       <c r="C139" s="1">
         <v>8.8313149896239087E-3</v>
       </c>
-      <c r="D139">
-        <v>14.8</v>
-      </c>
-      <c r="E139">
-        <v>84.565967293903057</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>13.8</v>
       </c>
@@ -2790,14 +1948,8 @@
       <c r="C140" s="1">
         <v>9.2613684537093937E-3</v>
       </c>
-      <c r="D140">
-        <v>14.9</v>
-      </c>
-      <c r="E140">
-        <v>74.633358258332606</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>13.9</v>
       </c>
@@ -2807,14 +1959,8 @@
       <c r="C141" s="1">
         <v>9.394103787288664E-3</v>
       </c>
-      <c r="D141">
-        <v>15</v>
-      </c>
-      <c r="E141">
-        <v>69.869968783345342</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>14</v>
       </c>
@@ -2824,14 +1970,8 @@
       <c r="C142" s="1">
         <v>9.511823058263584E-3</v>
       </c>
-      <c r="D142">
-        <v>15.1</v>
-      </c>
-      <c r="E142">
-        <v>67.557244698961711</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>14.1</v>
       </c>
@@ -2841,14 +1981,8 @@
       <c r="C143" s="1">
         <v>9.6211452826074871E-3</v>
       </c>
-      <c r="D143">
-        <v>15.2</v>
-      </c>
-      <c r="E143">
-        <v>66.89781629080619</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>14.2</v>
       </c>
@@ -2858,14 +1992,8 @@
       <c r="C144" s="1">
         <v>9.3532182819897978E-3</v>
       </c>
-      <c r="D144">
-        <v>15.3</v>
-      </c>
-      <c r="E144">
-        <v>66.141077419915774</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>14.3</v>
       </c>
@@ -2875,14 +2003,8 @@
       <c r="C145" s="1">
         <v>9.0710212460914617E-3</v>
       </c>
-      <c r="D145">
-        <v>15.4</v>
-      </c>
-      <c r="E145">
-        <v>60.370957349435088</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>14.4</v>
       </c>
@@ -2892,14 +2014,8 @@
       <c r="C146" s="1">
         <v>8.7782520824585906E-3</v>
       </c>
-      <c r="D146">
-        <v>15.5</v>
-      </c>
-      <c r="E146">
-        <v>60.831369924661139</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>14.5</v>
       </c>
@@ -2909,14 +2025,8 @@
       <c r="C147" s="1">
         <v>8.4919068041566879E-3</v>
       </c>
-      <c r="D147">
-        <v>15.6</v>
-      </c>
-      <c r="E147">
-        <v>75.456023576206618</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>14.6</v>
       </c>
@@ -2926,14 +2036,8 @@
       <c r="C148" s="1">
         <v>8.1210191497048355E-3</v>
       </c>
-      <c r="D148">
-        <v>15.7</v>
-      </c>
-      <c r="E148">
-        <v>94.887561618183454</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>14.7</v>
       </c>
@@ -2943,14 +2047,8 @@
       <c r="C149" s="1">
         <v>7.6084931948482036E-3</v>
       </c>
-      <c r="D149">
-        <v>15.8</v>
-      </c>
-      <c r="E149">
-        <v>68.279684701028472</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>14.8</v>
       </c>
@@ -2960,14 +2058,8 @@
       <c r="C150" s="1">
         <v>7.2889628279638038E-3</v>
       </c>
-      <c r="D150">
-        <v>15.9</v>
-      </c>
-      <c r="E150">
-        <v>71.193986598194329</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>14.9</v>
       </c>
@@ -2977,14 +2069,8 @@
       <c r="C151" s="1">
         <v>7.0976911323959524E-3</v>
       </c>
-      <c r="D151">
-        <v>16</v>
-      </c>
-      <c r="E151">
-        <v>75.975192966038449</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>15</v>
       </c>
@@ -2994,14 +2080,8 @@
       <c r="C152" s="1">
         <v>7.2185703775433704E-3</v>
       </c>
-      <c r="D152">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="E152">
-        <v>80.689754608043458</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>15.1</v>
       </c>
@@ -3011,14 +2091,8 @@
       <c r="C153">
         <v>7.2967599156929094E-3</v>
       </c>
-      <c r="D153">
-        <v>16.2</v>
-      </c>
-      <c r="E153">
-        <v>82.799990795821728</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>15.2</v>
       </c>
@@ -3028,14 +2102,8 @@
       <c r="C154">
         <v>7.0160901062526638E-3</v>
       </c>
-      <c r="D154">
-        <v>16.3</v>
-      </c>
-      <c r="E154">
-        <v>82.99556372043071</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>15.3</v>
       </c>
@@ -3045,14 +2113,8 @@
       <c r="C155">
         <v>7.2746090539204727E-3</v>
       </c>
-      <c r="D155">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="E155">
-        <v>79.85580667351411</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>15.4</v>
       </c>
@@ -3062,14 +2124,8 @@
       <c r="C156">
         <v>7.6302287457325722E-3</v>
       </c>
-      <c r="D156">
-        <v>16.5</v>
-      </c>
-      <c r="E156">
-        <v>82.068156037475049</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>15.5</v>
       </c>
@@ -3079,14 +2135,8 @@
       <c r="C157">
         <v>7.7520103634242509E-3</v>
       </c>
-      <c r="D157">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="E157">
-        <v>97.572897467846403</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>15.6</v>
       </c>
@@ -3096,14 +2146,8 @@
       <c r="C158">
         <v>8.1226210733424727E-3</v>
       </c>
-      <c r="D158">
-        <v>16.7</v>
-      </c>
-      <c r="E158">
-        <v>107.36394588029253</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>15.7</v>
       </c>
@@ -3113,14 +2157,8 @@
       <c r="C159">
         <v>8.0515109410820313E-3</v>
       </c>
-      <c r="D159">
-        <v>16.8</v>
-      </c>
-      <c r="E159">
-        <v>74.133253509289887</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>15.8</v>
       </c>
@@ -3130,14 +2168,8 @@
       <c r="C160">
         <v>8.4969043746389861E-3</v>
       </c>
-      <c r="D160">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="E160">
-        <v>75.378543725387942</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>15.9</v>
       </c>
@@ -3147,14 +2179,8 @@
       <c r="C161">
         <v>8.6886330577831145E-3</v>
       </c>
-      <c r="D161">
-        <v>17</v>
-      </c>
-      <c r="E161">
-        <v>75.091909986237113</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>16</v>
       </c>
@@ -3164,14 +2190,8 @@
       <c r="C162">
         <v>8.9895987644790024E-3</v>
       </c>
-      <c r="D162">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="E162">
-        <v>75.416452945133159</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>16.100000000000001</v>
       </c>
@@ -3181,14 +2201,8 @@
       <c r="C163">
         <v>9.4031035215539818E-3</v>
       </c>
-      <c r="D163">
-        <v>17.2</v>
-      </c>
-      <c r="E163">
-        <v>75.744339832437333</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>16.2</v>
       </c>
@@ -3198,14 +2212,8 @@
       <c r="C164">
         <v>9.5510597228081057E-3</v>
       </c>
-      <c r="D164">
-        <v>17.3</v>
-      </c>
-      <c r="E164">
-        <v>76.186964198464182</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>16.3</v>
       </c>
@@ -3215,14 +2223,8 @@
       <c r="C165">
         <v>9.6808551504404625E-3</v>
       </c>
-      <c r="D165">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="E165">
-        <v>71.512623135491808</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>16.399999999999999</v>
       </c>
@@ -3232,14 +2234,8 @@
       <c r="C166">
         <v>9.8112636391351864E-3</v>
       </c>
-      <c r="D166">
-        <v>17.5</v>
-      </c>
-      <c r="E166">
-        <v>73.16147296748025</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>16.5</v>
       </c>
@@ -3249,14 +2245,8 @@
       <c r="C167">
         <v>9.9387386286148537E-3</v>
       </c>
-      <c r="D167">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="E167">
-        <v>85.454179856820602</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>16.600000000000001</v>
       </c>
@@ -3266,14 +2256,8 @@
       <c r="C168">
         <v>9.4933805365595425E-3</v>
       </c>
-      <c r="D168">
-        <v>17.7</v>
-      </c>
-      <c r="E168">
-        <v>71.09949475872763</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>16.7</v>
       </c>
@@ -3283,14 +2267,8 @@
       <c r="C169">
         <v>9.3377460270605908E-3</v>
       </c>
-      <c r="D169">
-        <v>17.8</v>
-      </c>
-      <c r="E169">
-        <v>44.742276491250813</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>16.8</v>
       </c>
@@ -3300,14 +2278,8 @@
       <c r="C170">
         <v>9.3323229377589249E-3</v>
       </c>
-      <c r="D170">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="E170">
-        <v>50.162252617427448</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>16.899999999999999</v>
       </c>
@@ -3317,14 +2289,8 @@
       <c r="C171">
         <v>9.1049668932793246E-3</v>
       </c>
-      <c r="D171">
-        <v>18</v>
-      </c>
-      <c r="E171">
-        <v>50.434801227358328</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>17</v>
       </c>
@@ -3334,14 +2300,8 @@
       <c r="C172">
         <v>9.2152483924748535E-3</v>
       </c>
-      <c r="D172">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="E172">
-        <v>50.406419214488274</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>17.100000000000001</v>
       </c>
@@ -3351,14 +2311,8 @@
       <c r="C173">
         <v>9.1231749543808725E-3</v>
       </c>
-      <c r="D173">
-        <v>18.2</v>
-      </c>
-      <c r="E173">
-        <v>49.775872861444732</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>17.2</v>
       </c>
@@ -3368,14 +2322,8 @@
       <c r="C174">
         <v>8.9575767436081144E-3</v>
       </c>
-      <c r="D174">
-        <v>18.3</v>
-      </c>
-      <c r="E174">
-        <v>48.89440584789088</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>17.3</v>
       </c>
@@ -3385,14 +2333,8 @@
       <c r="C175">
         <v>9.0570874247412371E-3</v>
       </c>
-      <c r="D175">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="E175">
-        <v>43.830518006629603</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>17.399999999999999</v>
       </c>
@@ -3402,14 +2344,8 @@
       <c r="C176">
         <v>9.1955887379092851E-3</v>
       </c>
-      <c r="D176">
-        <v>18.5</v>
-      </c>
-      <c r="E176">
-        <v>43.830518006629603</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>17.5</v>
       </c>
@@ -3419,14 +2355,8 @@
       <c r="C177">
         <v>9.3355548164795205E-3</v>
       </c>
-      <c r="D177">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="E177">
-        <v>40.714883761226837</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>17.600000000000001</v>
       </c>
@@ -3436,14 +2366,8 @@
       <c r="C178">
         <v>9.8697859544836439E-3</v>
       </c>
-      <c r="D178">
-        <v>18.7</v>
-      </c>
-      <c r="E178">
-        <v>26.14235993076684</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>17.7</v>
       </c>
@@ -3453,14 +2377,8 @@
       <c r="C179">
         <v>1.00043953167366E-2</v>
       </c>
-      <c r="D179">
-        <v>18.8</v>
-      </c>
-      <c r="E179">
-        <v>24.217483109526469</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>17.8</v>
       </c>
@@ -3470,14 +2388,8 @@
       <c r="C180">
         <v>1.0610161222934469E-2</v>
       </c>
-      <c r="D180">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="E180">
-        <v>29.611067087183059</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>17.899999999999999</v>
       </c>
@@ -3487,14 +2399,8 @@
       <c r="C181">
         <v>1.088535716083595E-2</v>
       </c>
-      <c r="D181">
-        <v>19</v>
-      </c>
-      <c r="E181">
-        <v>28.943679586413136</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>18</v>
       </c>
@@ -3504,14 +2410,8 @@
       <c r="C182">
         <v>1.149157974840744E-2</v>
       </c>
-      <c r="D182">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="E182">
-        <v>26.761418550149379</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>18.100000000000001</v>
       </c>
@@ -3521,14 +2421,8 @@
       <c r="C183">
         <v>1.199873898142626E-2</v>
       </c>
-      <c r="D183">
-        <v>19.2</v>
-      </c>
-      <c r="E183">
-        <v>26.052445527892029</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>18.2</v>
       </c>
@@ -3538,14 +2432,8 @@
       <c r="C184">
         <v>1.235384392629587E-2</v>
       </c>
-      <c r="D184">
-        <v>19.3</v>
-      </c>
-      <c r="E184">
-        <v>25.833089508754622</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>18.3</v>
       </c>
@@ -3555,14 +2443,8 @@
       <c r="C185">
         <v>1.3010741813368641E-2</v>
       </c>
-      <c r="D185">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="E185">
-        <v>21.67210799299928</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>18.399999999999999</v>
       </c>
@@ -3572,14 +2454,8 @@
       <c r="C186">
         <v>1.373268393191289E-2</v>
       </c>
-      <c r="D186">
-        <v>19.5</v>
-      </c>
-      <c r="E186">
-        <v>23.136371857675066</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>18.5</v>
       </c>
@@ -3589,14 +2465,8 @@
       <c r="C187">
         <v>1.4443175786515329E-2</v>
       </c>
-      <c r="D187">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="E187">
-        <v>28.919200618427034</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>18.600000000000001</v>
       </c>
@@ -3606,14 +2476,8 @@
       <c r="C188">
         <v>1.4868565421953009E-2</v>
       </c>
-      <c r="D188">
-        <v>19.7</v>
-      </c>
-      <c r="E188">
-        <v>34.636454545190595</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>18.7</v>
       </c>
@@ -3623,14 +2487,8 @@
       <c r="C189">
         <v>1.5687280643581249E-2</v>
       </c>
-      <c r="D189">
-        <v>19.8</v>
-      </c>
-      <c r="E189">
-        <v>36.56802064510304</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>18.8</v>
       </c>
@@ -3640,14 +2498,8 @@
       <c r="C190">
         <v>1.6482023323892449E-2</v>
       </c>
-      <c r="D190">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="E190">
-        <v>40.994696885095991</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>18.899999999999999</v>
       </c>
@@ -3657,14 +2509,8 @@
       <c r="C191">
         <v>1.681592406845607E-2</v>
       </c>
-      <c r="D191">
-        <v>20</v>
-      </c>
-      <c r="E191">
-        <v>39.815066017258999</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>19</v>
       </c>
@@ -3674,14 +2520,8 @@
       <c r="C192">
         <v>1.734497005949015E-2</v>
       </c>
-      <c r="D192">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="E192">
-        <v>38.840961341818556</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>19.100000000000001</v>
       </c>
@@ -3691,14 +2531,8 @@
       <c r="C193">
         <v>1.7997329922285778E-2</v>
       </c>
-      <c r="D193">
-        <v>20.2</v>
-      </c>
-      <c r="E193">
-        <v>38.299196915164138</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>19.2</v>
       </c>
@@ -3708,14 +2542,8 @@
       <c r="C194">
         <v>1.8195411165135851E-2</v>
       </c>
-      <c r="D194">
-        <v>20.3</v>
-      </c>
-      <c r="E194">
-        <v>37.756452472243772</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>19.3</v>
       </c>
@@ -3725,14 +2553,8 @@
       <c r="C195">
         <v>1.881890100288661E-2</v>
       </c>
-      <c r="D195">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="E195">
-        <v>35.714769737158235</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>19.399999999999999</v>
       </c>
@@ -3742,14 +2564,8 @@
       <c r="C196">
         <v>1.9431979255617869E-2</v>
       </c>
-      <c r="D196">
-        <v>20.5</v>
-      </c>
-      <c r="E196">
-        <v>38.639097961698049</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>19.5</v>
       </c>
@@ -3759,14 +2575,8 @@
       <c r="C197">
         <v>1.992177124559338E-2</v>
       </c>
-      <c r="D197">
-        <v>20.6</v>
-      </c>
-      <c r="E197">
-        <v>46.967112390020596</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>19.600000000000001</v>
       </c>
@@ -3776,14 +2586,8 @@
       <c r="C198">
         <v>2.0442534454331619E-2</v>
       </c>
-      <c r="D198">
-        <v>20.7</v>
-      </c>
-      <c r="E198">
-        <v>54.192718968550736</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>19.7</v>
       </c>
@@ -3793,14 +2597,8 @@
       <c r="C199">
         <v>2.0453073063481458E-2</v>
       </c>
-      <c r="D199">
-        <v>20.8</v>
-      </c>
-      <c r="E199">
-        <v>52.247979865988803</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>19.8</v>
       </c>
@@ -3810,14 +2608,8 @@
       <c r="C200">
         <v>2.1092395439124941E-2</v>
       </c>
-      <c r="D200">
-        <v>20.9</v>
-      </c>
-      <c r="E200">
-        <v>54.924344223103482</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>19.899999999999999</v>
       </c>
@@ -3827,14 +2619,8 @@
       <c r="C201">
         <v>2.1220334015408699E-2</v>
       </c>
-      <c r="D201">
-        <v>21</v>
-      </c>
-      <c r="E201">
-        <v>54.530923602930557</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>20</v>
       </c>
@@ -3844,14 +2630,8 @@
       <c r="C202">
         <v>2.1840867983036239E-2</v>
       </c>
-      <c r="D202">
-        <v>21.1</v>
-      </c>
-      <c r="E202">
-        <v>54.010195885189702</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>20.100000000000001</v>
       </c>
@@ -3861,14 +2641,8 @@
       <c r="C203">
         <v>2.2142878735066759E-2</v>
       </c>
-      <c r="D203">
-        <v>21.2</v>
-      </c>
-      <c r="E203">
-        <v>53.767989160611471</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>20.2</v>
       </c>
@@ -3878,14 +2652,8 @@
       <c r="C204">
         <v>2.2699724438389669E-2</v>
       </c>
-      <c r="D204">
-        <v>21.3</v>
-      </c>
-      <c r="E204">
-        <v>54.659653709242619</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>20.3</v>
       </c>
@@ -3895,14 +2663,8 @@
       <c r="C205">
         <v>2.333070799042021E-2</v>
       </c>
-      <c r="D205">
-        <v>21.4</v>
-      </c>
-      <c r="E205">
-        <v>52.74865131301722</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>20.399999999999999</v>
       </c>
@@ -3912,14 +2674,8 @@
       <c r="C206">
         <v>2.3615909799571969E-2</v>
       </c>
-      <c r="D206">
-        <v>21.5</v>
-      </c>
-      <c r="E206">
-        <v>55.571004346637707</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>20.5</v>
       </c>
@@ -3929,14 +2685,8 @@
       <c r="C207">
         <v>2.433576131281601E-2</v>
       </c>
-      <c r="D207">
-        <v>21.6</v>
-      </c>
-      <c r="E207">
-        <v>60.127827914354725</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>20.6</v>
       </c>
@@ -3946,14 +2696,8 @@
       <c r="C208">
         <v>2.4474160744422241E-2</v>
       </c>
-      <c r="D208">
-        <v>21.7</v>
-      </c>
-      <c r="E208">
-        <v>57.588458190589975</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>20.7</v>
       </c>
@@ -3963,14 +2707,8 @@
       <c r="C209">
         <v>2.3872669599431979E-2</v>
       </c>
-      <c r="D209">
-        <v>21.8</v>
-      </c>
-      <c r="E209">
-        <v>49.622536012507538</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>20.8</v>
       </c>
@@ -3980,14 +2718,8 @@
       <c r="C210">
         <v>2.430020457207966E-2</v>
       </c>
-      <c r="D210">
-        <v>21.9</v>
-      </c>
-      <c r="E210">
-        <v>45.850021188305909</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>20.9</v>
       </c>
@@ -3997,14 +2729,8 @@
       <c r="C211">
         <v>2.502868274065213E-2</v>
       </c>
-      <c r="D211">
-        <v>22</v>
-      </c>
-      <c r="E211">
-        <v>41.242090731278786</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>21</v>
       </c>
@@ -4014,14 +2740,8 @@
       <c r="C212">
         <v>2.571590584670054E-2</v>
       </c>
-      <c r="D212">
-        <v>22.1</v>
-      </c>
-      <c r="E212">
-        <v>38.747696284589011</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>21.1</v>
       </c>
@@ -4031,14 +2751,8 @@
       <c r="C213">
         <v>2.6427010434337199E-2</v>
       </c>
-      <c r="D213">
-        <v>22.2</v>
-      </c>
-      <c r="E213">
-        <v>37.698221215426081</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>21.2</v>
       </c>
@@ -4048,14 +2762,8 @@
       <c r="C214">
         <v>2.7164426095724239E-2</v>
       </c>
-      <c r="D214">
-        <v>22.3</v>
-      </c>
-      <c r="E214">
-        <v>37.477568206116786</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>21.3</v>
       </c>
@@ -4065,14 +2773,8 @@
       <c r="C215">
         <v>2.8158183215137449E-2</v>
       </c>
-      <c r="D215">
-        <v>22.4</v>
-      </c>
-      <c r="E215">
-        <v>36.59485292714178</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>21.4</v>
       </c>
@@ -4082,14 +2784,8 @@
       <c r="C216">
         <v>2.910869962355369E-2</v>
       </c>
-      <c r="D216">
-        <v>22.5</v>
-      </c>
-      <c r="E216">
-        <v>38.852185024413124</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>21.5</v>
       </c>
@@ -4099,14 +2795,8 @@
       <c r="C217">
         <v>2.9795444020981918E-2</v>
       </c>
-      <c r="D217">
-        <v>22.6</v>
-      </c>
-      <c r="E217">
-        <v>40.633608236931785</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>21.6</v>
       </c>
@@ -4116,14 +2806,8 @@
       <c r="C218">
         <v>3.0228185840321529E-2</v>
       </c>
-      <c r="D218">
-        <v>22.7</v>
-      </c>
-      <c r="E218">
-        <v>35.018215002009839</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>21.7</v>
       </c>
@@ -4133,14 +2817,8 @@
       <c r="C219">
         <v>2.999453332486169E-2</v>
       </c>
-      <c r="D219">
-        <v>22.8</v>
-      </c>
-      <c r="E219">
-        <v>27.765306432776253</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>21.8</v>
       </c>
@@ -4150,14 +2828,8 @@
       <c r="C220">
         <v>3.0658095919356861E-2</v>
       </c>
-      <c r="D220">
-        <v>22.9</v>
-      </c>
-      <c r="E220">
-        <v>27.106239704475705</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>21.9</v>
       </c>
@@ -4167,14 +2839,8 @@
       <c r="C221">
         <v>3.1829429421893152E-2</v>
       </c>
-      <c r="D221">
-        <v>23</v>
-      </c>
-      <c r="E221">
-        <v>31.732078040992203</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>22</v>
       </c>
@@ -4184,14 +2850,8 @@
       <c r="C222">
         <v>3.4140697101972137E-2</v>
       </c>
-      <c r="D222">
-        <v>23.1</v>
-      </c>
-      <c r="E222">
-        <v>35.997359467669895</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>22.1</v>
       </c>
@@ -4201,14 +2861,8 @@
       <c r="C223">
         <v>3.5524488552135983E-2</v>
       </c>
-      <c r="D223">
-        <v>23.2</v>
-      </c>
-      <c r="E223">
-        <v>38.539374691557924</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>22.2</v>
       </c>
@@ -4218,14 +2872,8 @@
       <c r="C224">
         <v>3.6637526596844203E-2</v>
       </c>
-      <c r="D224">
-        <v>23.3</v>
-      </c>
-      <c r="E224">
-        <v>39.817697377411776</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>22.3</v>
       </c>
@@ -4235,14 +2883,8 @@
       <c r="C225">
         <v>3.7263702737356602E-2</v>
       </c>
-      <c r="D225">
-        <v>23.4</v>
-      </c>
-      <c r="E225">
-        <v>38.834959259463965</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>22.4</v>
       </c>
@@ -4252,14 +2894,8 @@
       <c r="C226">
         <v>3.7798380379557427E-2</v>
       </c>
-      <c r="D226">
-        <v>23.5</v>
-      </c>
-      <c r="E226">
-        <v>42.787186320021753</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>22.5</v>
       </c>
@@ -4269,14 +2905,8 @@
       <c r="C227">
         <v>3.8200292516264257E-2</v>
       </c>
-      <c r="D227">
-        <v>23.6</v>
-      </c>
-      <c r="E227">
-        <v>48.800541147397304</v>
-      </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>22.6</v>
       </c>
@@ -4286,14 +2916,8 @@
       <c r="C228">
         <v>3.7008170245475272E-2</v>
       </c>
-      <c r="D228">
-        <v>23.7</v>
-      </c>
-      <c r="E228">
-        <v>51.922242460778534</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>22.7</v>
       </c>
@@ -4303,14 +2927,8 @@
       <c r="C229">
         <v>3.7368518533452279E-2</v>
       </c>
-      <c r="D229">
-        <v>23.8</v>
-      </c>
-      <c r="E229">
-        <v>59.027336228925947</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>22.8</v>
       </c>
@@ -4320,14 +2938,8 @@
       <c r="C230">
         <v>3.8396994118489389E-2</v>
       </c>
-      <c r="D230">
-        <v>23.9</v>
-      </c>
-      <c r="E230">
-        <v>65.492182867862397</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>22.9</v>
       </c>
@@ -4337,14 +2949,8 @@
       <c r="C231">
         <v>3.8288899868713408E-2</v>
       </c>
-      <c r="D231">
-        <v>24</v>
-      </c>
-      <c r="E231">
-        <v>67.572853209063211</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>23</v>
       </c>
@@ -4354,14 +2960,8 @@
       <c r="C232">
         <v>3.772483172761773E-2</v>
       </c>
-      <c r="D232">
-        <v>24.1</v>
-      </c>
-      <c r="E232">
-        <v>69.313409483635098</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>23.1</v>
       </c>
@@ -4371,14 +2971,8 @@
       <c r="C233">
         <v>3.7245973521103599E-2</v>
       </c>
-      <c r="D233">
-        <v>24.2</v>
-      </c>
-      <c r="E233">
-        <v>71.451529779715571</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>23.2</v>
       </c>
@@ -4388,14 +2982,8 @@
       <c r="C234">
         <v>3.6685991873996182E-2</v>
       </c>
-      <c r="D234">
-        <v>24.3</v>
-      </c>
-      <c r="E234">
-        <v>73.812073064560366</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>23.3</v>
       </c>
@@ -4405,14 +2993,8 @@
       <c r="C235">
         <v>3.5984103830795117E-2</v>
       </c>
-      <c r="D235">
-        <v>24.4</v>
-      </c>
-      <c r="E235">
-        <v>76.842913135769692</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>23.4</v>
       </c>
@@ -4422,14 +3004,8 @@
       <c r="C236">
         <v>3.5462625563169273E-2</v>
       </c>
-      <c r="D236">
-        <v>24.5</v>
-      </c>
-      <c r="E236">
-        <v>83.786641053180489</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>23.5</v>
       </c>
@@ -4439,14 +3015,8 @@
       <c r="C237">
         <v>3.4790302373299893E-2</v>
       </c>
-      <c r="D237">
-        <v>24.6</v>
-      </c>
-      <c r="E237">
-        <v>86.89551734252133</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>23.6</v>
       </c>
@@ -4456,14 +3026,8 @@
       <c r="C238">
         <v>3.2433252980364993E-2</v>
       </c>
-      <c r="D238">
-        <v>24.7</v>
-      </c>
-      <c r="E238">
-        <v>86.187267130979492</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>23.7</v>
       </c>
@@ -4473,14 +3037,8 @@
       <c r="C239">
         <v>3.038312796999321E-2</v>
       </c>
-      <c r="D239">
-        <v>24.8</v>
-      </c>
-      <c r="E239">
-        <v>83.664665596335439</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>23.8</v>
       </c>
@@ -4490,14 +3048,8 @@
       <c r="C240">
         <v>2.8345371479740492E-2</v>
       </c>
-      <c r="D240">
-        <v>24.9</v>
-      </c>
-      <c r="E240">
-        <v>80.627087139763674</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>23.9</v>
       </c>
@@ -4507,14 +3059,8 @@
       <c r="C241">
         <v>2.7323588154987598E-2</v>
       </c>
-      <c r="D241">
-        <v>25</v>
-      </c>
-      <c r="E241">
-        <v>80.09863981003879</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>24</v>
       </c>
@@ -4525,7 +3071,7 @@
         <v>2.680167245975492E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>24.1</v>
       </c>
@@ -4536,7 +3082,7 @@
         <v>2.6043842199607731E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>24.2</v>
       </c>
@@ -4547,7 +3093,7 @@
         <v>2.5427017880527071E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>24.3</v>
       </c>
@@ -4558,7 +3104,7 @@
         <v>2.503648375140774E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>24.4</v>
       </c>
@@ -4569,7 +3115,7 @@
         <v>2.4279144879683551E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>24.5</v>
       </c>
@@ -4580,7 +3126,7 @@
         <v>2.3267498120673521E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>24.6</v>
       </c>
@@ -4591,7 +3137,7 @@
         <v>2.227970858789741E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>24.7</v>
       </c>
@@ -4602,7 +3148,7 @@
         <v>2.1242659023816359E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>24.8</v>
       </c>
@@ -4613,7 +3159,7 @@
         <v>2.0473676037175141E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>24.9</v>
       </c>
@@ -4624,7 +3170,7 @@
         <v>1.971590617715856E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'algae' of https://github.com/QSD-Group/EXPOsan into algae""
This reverts commit 79fd8a28e366cf636a379e7fafedf5abdd848685.
</commit_message>
<xml_diff>
--- a/exposan/pm2_ecorecover/data/dynamic_simul_result_calibration.xlsx
+++ b/exposan/pm2_ecorecover/data/dynamic_simul_result_calibration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Downloads\EXPOsan\exposan\pm2_ecorecover\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{904F1481-6EDE-48E0-91AF-6FDF1488E6C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985C642C-754F-4E63-B05B-204235C2E47C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{DEEFF93F-8712-407E-800A-077FF6958EEC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>t_stamp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,6 +36,14 @@
   </si>
   <si>
     <t>SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yield_1d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_stamp_yield</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -401,15 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47DDD832-617E-423B-B3BC-9FD3F4E9EB72}">
-  <dimension ref="A1:C252"/>
+  <dimension ref="A1:E252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A252"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,8 +427,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -430,8 +444,14 @@
       <c r="C2" s="1">
         <v>0.35744153755741681</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E2">
+        <v>141.22641287052892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -441,8 +461,14 @@
       <c r="C3" s="1">
         <v>1.107531976471491E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+      <c r="E3">
+        <v>135.97279294533516</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.2</v>
       </c>
@@ -452,8 +478,14 @@
       <c r="C4" s="1">
         <v>8.023750326828151E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1.3</v>
+      </c>
+      <c r="E4">
+        <v>137.25611599582237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.3</v>
       </c>
@@ -463,8 +495,14 @@
       <c r="C5" s="1">
         <v>8.3368790863734953E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>1.4</v>
+      </c>
+      <c r="E5">
+        <v>141.4937078208886</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.4</v>
       </c>
@@ -474,8 +512,14 @@
       <c r="C6" s="1">
         <v>8.4525318869409678E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>1.5</v>
+      </c>
+      <c r="E6">
+        <v>146.22981559997456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -485,8 +529,14 @@
       <c r="C7" s="1">
         <v>8.2427629558514404E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>1.6</v>
+      </c>
+      <c r="E7">
+        <v>155.19516202553595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.60000000000000009</v>
       </c>
@@ -496,8 +546,14 @@
       <c r="C8" s="1">
         <v>8.047608090998748E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>1.7</v>
+      </c>
+      <c r="E8">
+        <v>164.48641289040361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.70000000000000007</v>
       </c>
@@ -507,8 +563,14 @@
       <c r="C9" s="1">
         <v>7.6928155733528526E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>1.8</v>
+      </c>
+      <c r="E9">
+        <v>162.94445964495671</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.8</v>
       </c>
@@ -518,8 +580,14 @@
       <c r="C10" s="1">
         <v>7.5928288121893429E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>1.9</v>
+      </c>
+      <c r="E10">
+        <v>166.38433793495579</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.9</v>
       </c>
@@ -529,8 +597,14 @@
       <c r="C11" s="1">
         <v>7.7011487317907162E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>171.90915255790085</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -540,8 +614,14 @@
       <c r="C12" s="1">
         <v>7.7124903485505016E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>2.1</v>
+      </c>
+      <c r="E12">
+        <v>185.10118651133465</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1.1000000000000001</v>
       </c>
@@ -551,8 +631,14 @@
       <c r="C13" s="1">
         <v>7.6850542823217946E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E13">
+        <v>194.07285149384563</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1.2</v>
       </c>
@@ -562,8 +648,14 @@
       <c r="C14" s="1">
         <v>7.5907843687077828E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E14">
+        <v>204.71501041834455</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1.3</v>
       </c>
@@ -573,8 +665,14 @@
       <c r="C15" s="1">
         <v>7.4713145778358223E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>2.4</v>
+      </c>
+      <c r="E15">
+        <v>218.07116024736308</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1.4</v>
       </c>
@@ -584,8 +682,14 @@
       <c r="C16" s="1">
         <v>7.4172540833685281E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>2.5</v>
+      </c>
+      <c r="E16">
+        <v>238.31941931582114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1.5</v>
       </c>
@@ -595,8 +699,14 @@
       <c r="C17" s="1">
         <v>7.1545651875343577E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>2.6</v>
+      </c>
+      <c r="E17">
+        <v>272.09624752272452</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1.6</v>
       </c>
@@ -606,8 +716,14 @@
       <c r="C18" s="1">
         <v>6.8176199738561108E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>2.7</v>
+      </c>
+      <c r="E18">
+        <v>307.41925825383117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1.7</v>
       </c>
@@ -617,8 +733,14 @@
       <c r="C19" s="1">
         <v>6.4030155962494471E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>2.8</v>
+      </c>
+      <c r="E19">
+        <v>311.20108197779354</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1.8</v>
       </c>
@@ -628,8 +750,14 @@
       <c r="C20" s="1">
         <v>6.1844623865160526E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>2.9</v>
+      </c>
+      <c r="E20">
+        <v>316.16888749769345</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1.9</v>
       </c>
@@ -639,8 +767,14 @@
       <c r="C21" s="1">
         <v>5.890199985453818E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>326.15154922902803</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -650,8 +784,14 @@
       <c r="C22" s="1">
         <v>5.6469543849011847E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>3.1</v>
+      </c>
+      <c r="E22">
+        <v>324.02324436213377</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2.1</v>
       </c>
@@ -661,8 +801,14 @@
       <c r="C23" s="1">
         <v>5.3266579662909798E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>3.2</v>
+      </c>
+      <c r="E23">
+        <v>315.57106974593427</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2.2000000000000002</v>
       </c>
@@ -672,8 +818,14 @@
       <c r="C24" s="1">
         <v>4.9245021171890301E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>3.3</v>
+      </c>
+      <c r="E24">
+        <v>305.0056768948071</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2.2999999999999998</v>
       </c>
@@ -683,8 +835,14 @@
       <c r="C25" s="1">
         <v>4.4682823813590924E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>3.4</v>
+      </c>
+      <c r="E25">
+        <v>296.98411351130693</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2.4</v>
       </c>
@@ -694,8 +852,14 @@
       <c r="C26" s="1">
         <v>4.1120777190817859E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>3.5</v>
+      </c>
+      <c r="E26">
+        <v>290.32990663325063</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2.5</v>
       </c>
@@ -705,8 +869,14 @@
       <c r="C27" s="1">
         <v>3.900444179544525E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>3.6</v>
+      </c>
+      <c r="E27">
+        <v>281.10983535961992</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2.6</v>
       </c>
@@ -716,8 +886,14 @@
       <c r="C28" s="1">
         <v>3.662563688739968E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>3.7</v>
+      </c>
+      <c r="E28">
+        <v>263.79042643133266</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2.7</v>
       </c>
@@ -727,8 +903,14 @@
       <c r="C29" s="1">
         <v>3.5054778851214912E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>3.8</v>
+      </c>
+      <c r="E29">
+        <v>217.35976430814989</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2.8</v>
       </c>
@@ -738,8 +920,14 @@
       <c r="C30" s="1">
         <v>3.4563613546098049E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>3.9</v>
+      </c>
+      <c r="E30">
+        <v>185.49583065482707</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2.9</v>
       </c>
@@ -749,8 +937,14 @@
       <c r="C31" s="1">
         <v>3.5341997975597739E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>164.67647430927929</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -760,8 +954,14 @@
       <c r="C32" s="1">
         <v>3.6180510852257151E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>4.1000000000000014</v>
+      </c>
+      <c r="E32">
+        <v>143.97381475632523</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3.1</v>
       </c>
@@ -771,8 +971,14 @@
       <c r="C33" s="1">
         <v>3.963679945281906E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <v>4.2</v>
+      </c>
+      <c r="E33">
+        <v>133.95044793283728</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3.2</v>
       </c>
@@ -782,8 +988,14 @@
       <c r="C34" s="1">
         <v>4.1607249923814628E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <v>4.3</v>
+      </c>
+      <c r="E34">
+        <v>128.69920570803458</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3.3</v>
       </c>
@@ -793,8 +1005,14 @@
       <c r="C35" s="1">
         <v>4.4811730158857681E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E35">
+        <v>125.82675414951444</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>3.4</v>
       </c>
@@ -804,8 +1022,14 @@
       <c r="C36" s="1">
         <v>4.9060457617201708E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <v>4.5</v>
+      </c>
+      <c r="E36">
+        <v>122.31902451577163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>3.5</v>
       </c>
@@ -815,8 +1039,14 @@
       <c r="C37" s="1">
         <v>5.375602114115423E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37">
+        <v>4.6000000000000014</v>
+      </c>
+      <c r="E37">
+        <v>119.08849859686953</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>3.6</v>
       </c>
@@ -826,8 +1056,14 @@
       <c r="C38" s="1">
         <v>5.7965711613269539E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <v>4.7</v>
+      </c>
+      <c r="E38">
+        <v>107.75993290630599</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3.7</v>
       </c>
@@ -837,8 +1073,14 @@
       <c r="C39" s="1">
         <v>6.1668751874600428E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39">
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="E39">
+        <v>80.454469551759615</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>3.8</v>
       </c>
@@ -848,8 +1090,14 @@
       <c r="C40" s="1">
         <v>6.7841741523916137E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E40">
+        <v>70.6610342144795</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>3.9</v>
       </c>
@@ -859,8 +1107,14 @@
       <c r="C41" s="1">
         <v>7.3934642554173398E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41">
+        <v>5</v>
+      </c>
+      <c r="E41">
+        <v>69.105060705339895</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>4</v>
       </c>
@@ -870,8 +1124,14 @@
       <c r="C42" s="1">
         <v>8.0319126961436119E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42">
+        <v>5.1000000000000014</v>
+      </c>
+      <c r="E42">
+        <v>67.769369182296799</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4.1000000000000014</v>
       </c>
@@ -881,8 +1141,14 @@
       <c r="C43" s="1">
         <v>8.7566441485514932E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43">
+        <v>5.2</v>
+      </c>
+      <c r="E43">
+        <v>66.622472229871377</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>4.2</v>
       </c>
@@ -892,8 +1158,14 @@
       <c r="C44" s="1">
         <v>9.340020468893314E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44">
+        <v>5.3000000000000007</v>
+      </c>
+      <c r="E44">
+        <v>65.734720727098164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>4.3</v>
       </c>
@@ -903,8 +1175,14 @@
       <c r="C45" s="1">
         <v>1.005687504009666E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45">
+        <v>5.4</v>
+      </c>
+      <c r="E45">
+        <v>66.91647524561543</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>4.4000000000000004</v>
       </c>
@@ -914,8 +1192,14 @@
       <c r="C46" s="1">
         <v>1.056710418044126E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <v>5.5</v>
+      </c>
+      <c r="E46">
+        <v>69.792775866637314</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4.5</v>
       </c>
@@ -925,8 +1209,14 @@
       <c r="C47" s="1">
         <v>1.1050850441609439E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <v>5.6000000000000014</v>
+      </c>
+      <c r="E47">
+        <v>71.999558753876386</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>4.6000000000000014</v>
       </c>
@@ -936,8 +1226,14 @@
       <c r="C48" s="1">
         <v>1.1393393895568831E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>5.7</v>
+      </c>
+      <c r="E48">
+        <v>69.889997832841473</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4.7</v>
       </c>
@@ -947,8 +1243,14 @@
       <c r="C49" s="1">
         <v>1.166064289197348E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="E49">
+        <v>62.205462418638056</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>4.8000000000000007</v>
       </c>
@@ -958,8 +1260,14 @@
       <c r="C50" s="1">
         <v>1.199332966342577E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <v>5.9</v>
+      </c>
+      <c r="E50">
+        <v>58.996395382408672</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>4.9000000000000004</v>
       </c>
@@ -969,8 +1277,14 @@
       <c r="C51" s="1">
         <v>1.226872553654202E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51">
+        <v>6</v>
+      </c>
+      <c r="E51">
+        <v>59.091189459017215</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>5</v>
       </c>
@@ -980,8 +1294,14 @@
       <c r="C52" s="1">
         <v>1.2707943516759209E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <v>6.1000000000000014</v>
+      </c>
+      <c r="E52">
+        <v>59.297671256470601</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5.1000000000000014</v>
       </c>
@@ -991,8 +1311,14 @@
       <c r="C53" s="1">
         <v>1.3117618006091E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53">
+        <v>6.2</v>
+      </c>
+      <c r="E53">
+        <v>59.666896195248796</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>5.2</v>
       </c>
@@ -1002,8 +1328,14 @@
       <c r="C54" s="1">
         <v>1.324983839921591E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54">
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="E54">
+        <v>60.169494063175463</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>5.3000000000000007</v>
       </c>
@@ -1013,8 +1345,14 @@
       <c r="C55" s="1">
         <v>1.364164342781549E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55">
+        <v>6.4</v>
+      </c>
+      <c r="E55">
+        <v>62.273426130964296</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>5.4</v>
       </c>
@@ -1024,8 +1362,14 @@
       <c r="C56" s="1">
         <v>1.369136083747537E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56">
+        <v>6.5</v>
+      </c>
+      <c r="E56">
+        <v>64.850657243796263</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>5.5</v>
       </c>
@@ -1035,8 +1379,14 @@
       <c r="C57" s="1">
         <v>1.391303899136772E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <v>6.6000000000000014</v>
+      </c>
+      <c r="E57">
+        <v>66.648301432291248</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>5.6000000000000014</v>
       </c>
@@ -1046,8 +1396,14 @@
       <c r="C58" s="1">
         <v>1.3763069438431389E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58">
+        <v>6.7</v>
+      </c>
+      <c r="E58">
+        <v>66.326706835516902</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>5.7</v>
       </c>
@@ -1057,8 +1413,14 @@
       <c r="C59" s="1">
         <v>1.387122135430891E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="E59">
+        <v>61.901482579563634</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>5.8000000000000007</v>
       </c>
@@ -1068,8 +1430,14 @@
       <c r="C60" s="1">
         <v>1.385835732877426E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>6.9</v>
+      </c>
+      <c r="E60">
+        <v>60.457148802318507</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>5.9</v>
       </c>
@@ -1079,8 +1447,14 @@
       <c r="C61" s="1">
         <v>1.4215790718244491E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>7</v>
+      </c>
+      <c r="E61">
+        <v>62.838532845573553</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>6</v>
       </c>
@@ -1090,8 +1464,14 @@
       <c r="C62" s="1">
         <v>1.4306328030382891E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62">
+        <v>7.1000000000000014</v>
+      </c>
+      <c r="E62">
+        <v>66.161927305941902</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>6.1000000000000014</v>
       </c>
@@ -1101,8 +1481,14 @@
       <c r="C63" s="1">
         <v>1.465699042511567E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D63">
+        <v>7.2</v>
+      </c>
+      <c r="E63">
+        <v>69.524153233279534</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>6.2</v>
       </c>
@@ -1112,8 +1498,14 @@
       <c r="C64" s="1">
         <v>1.4793210369891259E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64">
+        <v>7.3000000000000007</v>
+      </c>
+      <c r="E64">
+        <v>72.138253257486539</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>6.3000000000000007</v>
       </c>
@@ -1123,8 +1515,14 @@
       <c r="C65" s="1">
         <v>1.503102911195551E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65">
+        <v>7.4</v>
+      </c>
+      <c r="E65">
+        <v>75.030372357463406</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>6.4</v>
       </c>
@@ -1134,8 +1532,14 @@
       <c r="C66" s="1">
         <v>1.5295859825186719E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <v>7.5</v>
+      </c>
+      <c r="E66">
+        <v>78.366202266904381</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>6.5</v>
       </c>
@@ -1145,8 +1549,14 @@
       <c r="C67" s="1">
         <v>1.527187094526922E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <v>7.6000000000000014</v>
+      </c>
+      <c r="E67">
+        <v>80.690828485220308</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>6.6000000000000014</v>
       </c>
@@ -1156,8 +1566,14 @@
       <c r="C68" s="1">
         <v>1.5306904098264389E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>7.7</v>
+      </c>
+      <c r="E68">
+        <v>84.527857271848703</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>6.7</v>
       </c>
@@ -1167,8 +1583,14 @@
       <c r="C69" s="1">
         <v>1.5299679827600981E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <v>7.8000000000000007</v>
+      </c>
+      <c r="E69">
+        <v>79.56130898264756</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>6.8000000000000007</v>
       </c>
@@ -1178,8 +1600,14 @@
       <c r="C70" s="1">
         <v>1.5198612509803521E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70">
+        <v>7.9</v>
+      </c>
+      <c r="E70">
+        <v>71.996111088716148</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>6.9</v>
       </c>
@@ -1189,8 +1617,14 @@
       <c r="C71" s="1">
         <v>1.528280404432324E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>8</v>
+      </c>
+      <c r="E71">
+        <v>67.896267524560074</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>7</v>
       </c>
@@ -1200,8 +1634,14 @@
       <c r="C72" s="1">
         <v>1.5302512144562141E-2</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D72">
+        <v>8.1</v>
+      </c>
+      <c r="E72">
+        <v>66.181918062494347</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>7.1000000000000014</v>
       </c>
@@ -1211,8 +1651,14 @@
       <c r="C73" s="1">
         <v>1.5202374297606919E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <v>8.2000000000000011</v>
+      </c>
+      <c r="E73">
+        <v>64.035443585099245</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>7.2</v>
       </c>
@@ -1222,8 +1668,14 @@
       <c r="C74" s="1">
         <v>1.5050079679233139E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E74">
+        <v>62.062452959333221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>7.3000000000000007</v>
       </c>
@@ -1233,8 +1685,14 @@
       <c r="C75" s="1">
         <v>1.521206802512476E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>8.4</v>
+      </c>
+      <c r="E75">
+        <v>62.509860016672995</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>7.4</v>
       </c>
@@ -1244,8 +1702,14 @@
       <c r="C76" s="1">
         <v>1.554036744227931E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>8.5</v>
+      </c>
+      <c r="E76">
+        <v>64.361445104550242</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>7.5</v>
       </c>
@@ -1255,8 +1719,14 @@
       <c r="C77" s="1">
         <v>1.557397797271105E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77">
+        <v>8.6</v>
+      </c>
+      <c r="E77">
+        <v>67.97017108583151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>7.6000000000000014</v>
       </c>
@@ -1266,8 +1736,14 @@
       <c r="C78" s="1">
         <v>1.579028696060486E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78">
+        <v>8.7000000000000011</v>
+      </c>
+      <c r="E78">
+        <v>73.756488747295904</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>7.7</v>
       </c>
@@ -1277,8 +1753,14 @@
       <c r="C79" s="1">
         <v>1.544228227985996E-2</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E79">
+        <v>69.104290423400585</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>7.8000000000000007</v>
       </c>
@@ -1288,8 +1770,14 @@
       <c r="C80" s="1">
         <v>1.5649686977813351E-2</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>8.9</v>
+      </c>
+      <c r="E80">
+        <v>67.356434819572897</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>7.9</v>
       </c>
@@ -1299,8 +1787,14 @@
       <c r="C81" s="1">
         <v>1.5980002786042509E-2</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>9</v>
+      </c>
+      <c r="E81">
+        <v>72.006876520816348</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>8</v>
       </c>
@@ -1310,8 +1804,14 @@
       <c r="C82" s="1">
         <v>1.6729880685912229E-2</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>9.1</v>
+      </c>
+      <c r="E82">
+        <v>76.912306483218003</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>8.1</v>
       </c>
@@ -1321,8 +1821,14 @@
       <c r="C83" s="1">
         <v>1.6759911977767449E-2</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>9.2000000000000011</v>
+      </c>
+      <c r="E83">
+        <v>78.595175802044309</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>8.2000000000000011</v>
       </c>
@@ -1332,8 +1838,14 @@
       <c r="C84" s="1">
         <v>1.67846543111933E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E84">
+        <v>80.106090167518261</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>8.3000000000000007</v>
       </c>
@@ -1343,8 +1855,14 @@
       <c r="C85" s="1">
         <v>1.6594358724505359E-2</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>9.4</v>
+      </c>
+      <c r="E85">
+        <v>83.524617936634399</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>8.4</v>
       </c>
@@ -1354,8 +1872,14 @@
       <c r="C86" s="1">
         <v>1.6344963736168679E-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>9.5</v>
+      </c>
+      <c r="E86">
+        <v>88.966936865417466</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>8.5</v>
       </c>
@@ -1365,8 +1889,14 @@
       <c r="C87" s="1">
         <v>1.6002392676923591E-2</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="E87">
+        <v>93.385143939669902</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>8.6</v>
       </c>
@@ -1376,8 +1906,14 @@
       <c r="C88" s="1">
         <v>1.552642384107283E-2</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>9.7000000000000011</v>
+      </c>
+      <c r="E88">
+        <v>97.714759568979829</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>8.7000000000000011</v>
       </c>
@@ -1387,8 +1923,14 @@
       <c r="C89" s="1">
         <v>1.457597872810504E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E89">
+        <v>89.837050977472032</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>8.8000000000000007</v>
       </c>
@@ -1398,8 +1940,14 @@
       <c r="C90" s="1">
         <v>1.4167911938584561E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90">
+        <v>9.9</v>
+      </c>
+      <c r="E90">
+        <v>84.685777993895087</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>8.9</v>
       </c>
@@ -1409,8 +1957,14 @@
       <c r="C91" s="1">
         <v>1.39619055632788E-2</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <v>10</v>
+      </c>
+      <c r="E91">
+        <v>84.276444503853838</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>9</v>
       </c>
@@ -1420,8 +1974,14 @@
       <c r="C92" s="1">
         <v>1.371319055641233E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92">
+        <v>10.1</v>
+      </c>
+      <c r="E92">
+        <v>82.39011785191704</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>9.1</v>
       </c>
@@ -1431,8 +1991,14 @@
       <c r="C93" s="1">
         <v>1.3410869000320491E-2</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E93">
+        <v>82.192089179606214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>9.2000000000000011</v>
       </c>
@@ -1442,8 +2008,14 @@
       <c r="C94" s="1">
         <v>1.309901987120321E-2</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94">
+        <v>10.3</v>
+      </c>
+      <c r="E94">
+        <v>82.473039790810247</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>9.3000000000000007</v>
       </c>
@@ -1453,8 +2025,14 @@
       <c r="C95" s="1">
         <v>1.2785479007028099E-2</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95">
+        <v>10.4</v>
+      </c>
+      <c r="E95">
+        <v>83.736316238605241</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>9.4</v>
       </c>
@@ -1464,8 +2042,14 @@
       <c r="C96" s="1">
         <v>1.236175574158252E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D96">
+        <v>10.5</v>
+      </c>
+      <c r="E96">
+        <v>85.188818895842346</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>9.5</v>
       </c>
@@ -1475,8 +2059,14 @@
       <c r="C97" s="1">
         <v>1.1823278127276749E-2</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D97">
+        <v>10.6</v>
+      </c>
+      <c r="E97">
+        <v>84.269834050745573</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>9.6000000000000014</v>
       </c>
@@ -1486,8 +2076,14 @@
       <c r="C98" s="1">
         <v>1.139245045375299E-2</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D98">
+        <v>10.7</v>
+      </c>
+      <c r="E98">
+        <v>81.745703681267173</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>9.7000000000000011</v>
       </c>
@@ -1497,8 +2093,14 @@
       <c r="C99" s="1">
         <v>1.0919789190071199E-2</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D99">
+        <v>10.8</v>
+      </c>
+      <c r="E99">
+        <v>73.31680498787108</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>9.8000000000000007</v>
       </c>
@@ -1508,8 +2110,14 @@
       <c r="C100" s="1">
         <v>1.0540817049596189E-2</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D100">
+        <v>10.9</v>
+      </c>
+      <c r="E100">
+        <v>73.024892627670155</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>9.9</v>
       </c>
@@ -1519,8 +2127,14 @@
       <c r="C101" s="1">
         <v>1.025390064694965E-2</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D101">
+        <v>11</v>
+      </c>
+      <c r="E101">
+        <v>76.171723874362442</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>10</v>
       </c>
@@ -1530,8 +2144,14 @@
       <c r="C102" s="1">
         <v>9.9826400208533686E-3</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D102">
+        <v>11.1</v>
+      </c>
+      <c r="E102">
+        <v>79.731468800898838</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>10.1</v>
       </c>
@@ -1541,8 +2161,14 @@
       <c r="C103" s="1">
         <v>9.6883819608733143E-3</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D103">
+        <v>11.2</v>
+      </c>
+      <c r="E103">
+        <v>84.926117407681105</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>10.199999999999999</v>
       </c>
@@ -1552,8 +2178,14 @@
       <c r="C104" s="1">
         <v>9.2910202099324244E-3</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D104">
+        <v>11.3</v>
+      </c>
+      <c r="E104">
+        <v>88.196861862918013</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>10.3</v>
       </c>
@@ -1563,8 +2195,14 @@
       <c r="C105" s="1">
         <v>8.8389841353768046E-3</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D105">
+        <v>11.4</v>
+      </c>
+      <c r="E105">
+        <v>93.162862203673726</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>10.4</v>
       </c>
@@ -1574,8 +2212,14 @@
       <c r="C106" s="1">
         <v>8.3701684432845314E-3</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D106">
+        <v>11.5</v>
+      </c>
+      <c r="E106">
+        <v>103.4426825283621</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>10.5</v>
       </c>
@@ -1585,8 +2229,14 @@
       <c r="C107" s="1">
         <v>8.0773493100987238E-3</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D107">
+        <v>11.6</v>
+      </c>
+      <c r="E107">
+        <v>109.03260580205861</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>10.6</v>
       </c>
@@ -1596,8 +2246,14 @@
       <c r="C108" s="1">
         <v>7.7857282493948247E-3</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D108">
+        <v>11.7</v>
+      </c>
+      <c r="E108">
+        <v>113.72818004229948</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>10.7</v>
       </c>
@@ -1607,8 +2263,14 @@
       <c r="C109" s="1">
         <v>7.4779006302009791E-3</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D109">
+        <v>11.8</v>
+      </c>
+      <c r="E109">
+        <v>115.00859453318331</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>10.8</v>
       </c>
@@ -1618,8 +2280,14 @@
       <c r="C110" s="1">
         <v>7.2986977702901128E-3</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D110">
+        <v>11.9</v>
+      </c>
+      <c r="E110">
+        <v>114.76792465710119</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>10.9</v>
       </c>
@@ -1629,8 +2297,14 @@
       <c r="C111" s="1">
         <v>7.1549567989567789E-3</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D111">
+        <v>12</v>
+      </c>
+      <c r="E111">
+        <v>115.17166502180503</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>11</v>
       </c>
@@ -1640,8 +2314,14 @@
       <c r="C112" s="1">
         <v>6.9610729085756969E-3</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D112">
+        <v>12.1</v>
+      </c>
+      <c r="E112">
+        <v>116.01924680569674</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>11.1</v>
       </c>
@@ -1651,8 +2331,14 @@
       <c r="C113" s="1">
         <v>6.7900989115672744E-3</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D113">
+        <v>12.2</v>
+      </c>
+      <c r="E113">
+        <v>116.58742112065853</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>11.2</v>
       </c>
@@ -1662,8 +2348,14 @@
       <c r="C114" s="1">
         <v>6.8278936740797597E-3</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D114">
+        <v>12.3</v>
+      </c>
+      <c r="E114">
+        <v>117.28985356508851</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>11.3</v>
       </c>
@@ -1673,8 +2365,14 @@
       <c r="C115" s="1">
         <v>6.6296016918297312E-3</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D115">
+        <v>12.4</v>
+      </c>
+      <c r="E115">
+        <v>121.21788906979003</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>11.4</v>
       </c>
@@ -1684,8 +2382,14 @@
       <c r="C116" s="1">
         <v>6.6811396618864224E-3</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D116">
+        <v>12.5</v>
+      </c>
+      <c r="E116">
+        <v>130.51844692658599</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>11.5</v>
       </c>
@@ -1695,8 +2399,14 @@
       <c r="C117" s="1">
         <v>6.5243756549859134E-3</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D117">
+        <v>12.6</v>
+      </c>
+      <c r="E117">
+        <v>135.70093781055797</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>11.6</v>
       </c>
@@ -1706,8 +2416,14 @@
       <c r="C118" s="1">
         <v>6.4405641662449113E-3</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D118">
+        <v>12.7</v>
+      </c>
+      <c r="E118">
+        <v>143.88913505087058</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>11.7</v>
       </c>
@@ -1717,8 +2433,14 @@
       <c r="C119" s="1">
         <v>6.4784934559068523E-3</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D119">
+        <v>12.8</v>
+      </c>
+      <c r="E119">
+        <v>145.26423136997519</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>11.8</v>
       </c>
@@ -1728,8 +2450,14 @@
       <c r="C120" s="1">
         <v>6.325693973864753E-3</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D120">
+        <v>12.9</v>
+      </c>
+      <c r="E120">
+        <v>141.00582242427657</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>11.9</v>
       </c>
@@ -1739,8 +2467,14 @@
       <c r="C121" s="1">
         <v>6.3407840360676336E-3</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D121">
+        <v>13</v>
+      </c>
+      <c r="E121">
+        <v>140.58004266612076</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>12</v>
       </c>
@@ -1750,8 +2484,14 @@
       <c r="C122" s="1">
         <v>6.4335562604397418E-3</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D122">
+        <v>13.1</v>
+      </c>
+      <c r="E122">
+        <v>139.85438078728146</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>12.1</v>
       </c>
@@ -1761,8 +2501,14 @@
       <c r="C123" s="1">
         <v>6.2362993685006994E-3</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D123">
+        <v>13.2</v>
+      </c>
+      <c r="E123">
+        <v>138.42919754476924</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>12.2</v>
       </c>
@@ -1772,8 +2518,14 @@
       <c r="C124" s="1">
         <v>6.3025833835089872E-3</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D124">
+        <v>13.3</v>
+      </c>
+      <c r="E124">
+        <v>136.75807144930806</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>12.3</v>
       </c>
@@ -1783,8 +2535,14 @@
       <c r="C125" s="1">
         <v>6.3887410656872931E-3</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D125">
+        <v>13.4</v>
+      </c>
+      <c r="E125">
+        <v>136.33096750496463</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>12.4</v>
       </c>
@@ -1794,8 +2552,14 @@
       <c r="C126" s="1">
         <v>6.1514519382426646E-3</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D126">
+        <v>13.5</v>
+      </c>
+      <c r="E126">
+        <v>138.49194783720057</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>12.5</v>
       </c>
@@ -1805,8 +2569,14 @@
       <c r="C127" s="1">
         <v>6.1760566090801623E-3</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D127">
+        <v>13.6</v>
+      </c>
+      <c r="E127">
+        <v>136.93572900130602</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>12.6</v>
       </c>
@@ -1816,8 +2586,14 @@
       <c r="C128" s="1">
         <v>5.9427329344435391E-3</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D128">
+        <v>13.7</v>
+      </c>
+      <c r="E128">
+        <v>128.51617440954612</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>12.7</v>
       </c>
@@ -1827,8 +2603,14 @@
       <c r="C129" s="1">
         <v>5.9120398319980469E-3</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D129">
+        <v>13.8</v>
+      </c>
+      <c r="E129">
+        <v>115.34741378531913</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>12.8</v>
       </c>
@@ -1838,8 +2620,14 @@
       <c r="C130" s="1">
         <v>5.9660813791428836E-3</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D130">
+        <v>13.9</v>
+      </c>
+      <c r="E130">
+        <v>103.29798606292611</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>12.9</v>
       </c>
@@ -1849,8 +2637,14 @@
       <c r="C131" s="1">
         <v>6.0643245431174489E-3</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D131">
+        <v>14</v>
+      </c>
+      <c r="E131">
+        <v>101.11411408429127</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>13</v>
       </c>
@@ -1860,8 +2654,14 @@
       <c r="C132" s="1">
         <v>6.4882603096759724E-3</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D132">
+        <v>14.1</v>
+      </c>
+      <c r="E132">
+        <v>99.133180300042525</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>13.1</v>
       </c>
@@ -1871,8 +2671,14 @@
       <c r="C133" s="1">
         <v>6.6174701543940959E-3</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D133">
+        <v>14.2</v>
+      </c>
+      <c r="E133">
+        <v>97.597777919000819</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>13.2</v>
       </c>
@@ -1882,8 +2688,14 @@
       <c r="C134" s="1">
         <v>7.0581802478038164E-3</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D134">
+        <v>14.3</v>
+      </c>
+      <c r="E134">
+        <v>96.767501424670527</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>13.3</v>
       </c>
@@ -1893,8 +2705,14 @@
       <c r="C135" s="1">
         <v>7.505469630874553E-3</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D135">
+        <v>14.4</v>
+      </c>
+      <c r="E135">
+        <v>90.590565816466537</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>13.4</v>
       </c>
@@ -1904,8 +2722,14 @@
       <c r="C136" s="1">
         <v>7.9628694494917555E-3</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D136">
+        <v>14.5</v>
+      </c>
+      <c r="E136">
+        <v>84.297989863776309</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>13.5</v>
       </c>
@@ -1915,8 +2739,14 @@
       <c r="C137" s="1">
         <v>8.3662689757695204E-3</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D137">
+        <v>14.6</v>
+      </c>
+      <c r="E137">
+        <v>84.029982610536905</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>13.6</v>
       </c>
@@ -1926,8 +2756,14 @@
       <c r="C138" s="1">
         <v>8.7090820048649521E-3</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D138">
+        <v>14.7</v>
+      </c>
+      <c r="E138">
+        <v>96.256559634257712</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>13.7</v>
       </c>
@@ -1937,8 +2773,14 @@
       <c r="C139" s="1">
         <v>8.8313149896239087E-3</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D139">
+        <v>14.8</v>
+      </c>
+      <c r="E139">
+        <v>84.565967293903057</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>13.8</v>
       </c>
@@ -1948,8 +2790,14 @@
       <c r="C140" s="1">
         <v>9.2613684537093937E-3</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D140">
+        <v>14.9</v>
+      </c>
+      <c r="E140">
+        <v>74.633358258332606</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>13.9</v>
       </c>
@@ -1959,8 +2807,14 @@
       <c r="C141" s="1">
         <v>9.394103787288664E-3</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D141">
+        <v>15</v>
+      </c>
+      <c r="E141">
+        <v>69.869968783345342</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>14</v>
       </c>
@@ -1970,8 +2824,14 @@
       <c r="C142" s="1">
         <v>9.511823058263584E-3</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D142">
+        <v>15.1</v>
+      </c>
+      <c r="E142">
+        <v>67.557244698961711</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>14.1</v>
       </c>
@@ -1981,8 +2841,14 @@
       <c r="C143" s="1">
         <v>9.6211452826074871E-3</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D143">
+        <v>15.2</v>
+      </c>
+      <c r="E143">
+        <v>66.89781629080619</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>14.2</v>
       </c>
@@ -1992,8 +2858,14 @@
       <c r="C144" s="1">
         <v>9.3532182819897978E-3</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D144">
+        <v>15.3</v>
+      </c>
+      <c r="E144">
+        <v>66.141077419915774</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>14.3</v>
       </c>
@@ -2003,8 +2875,14 @@
       <c r="C145" s="1">
         <v>9.0710212460914617E-3</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D145">
+        <v>15.4</v>
+      </c>
+      <c r="E145">
+        <v>60.370957349435088</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>14.4</v>
       </c>
@@ -2014,8 +2892,14 @@
       <c r="C146" s="1">
         <v>8.7782520824585906E-3</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D146">
+        <v>15.5</v>
+      </c>
+      <c r="E146">
+        <v>60.831369924661139</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>14.5</v>
       </c>
@@ -2025,8 +2909,14 @@
       <c r="C147" s="1">
         <v>8.4919068041566879E-3</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D147">
+        <v>15.6</v>
+      </c>
+      <c r="E147">
+        <v>75.456023576206618</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>14.6</v>
       </c>
@@ -2036,8 +2926,14 @@
       <c r="C148" s="1">
         <v>8.1210191497048355E-3</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D148">
+        <v>15.7</v>
+      </c>
+      <c r="E148">
+        <v>94.887561618183454</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>14.7</v>
       </c>
@@ -2047,8 +2943,14 @@
       <c r="C149" s="1">
         <v>7.6084931948482036E-3</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D149">
+        <v>15.8</v>
+      </c>
+      <c r="E149">
+        <v>68.279684701028472</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>14.8</v>
       </c>
@@ -2058,8 +2960,14 @@
       <c r="C150" s="1">
         <v>7.2889628279638038E-3</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D150">
+        <v>15.9</v>
+      </c>
+      <c r="E150">
+        <v>71.193986598194329</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>14.9</v>
       </c>
@@ -2069,8 +2977,14 @@
       <c r="C151" s="1">
         <v>7.0976911323959524E-3</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D151">
+        <v>16</v>
+      </c>
+      <c r="E151">
+        <v>75.975192966038449</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>15</v>
       </c>
@@ -2080,8 +2994,14 @@
       <c r="C152" s="1">
         <v>7.2185703775433704E-3</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D152">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="E152">
+        <v>80.689754608043458</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>15.1</v>
       </c>
@@ -2091,8 +3011,14 @@
       <c r="C153">
         <v>7.2967599156929094E-3</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D153">
+        <v>16.2</v>
+      </c>
+      <c r="E153">
+        <v>82.799990795821728</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>15.2</v>
       </c>
@@ -2102,8 +3028,14 @@
       <c r="C154">
         <v>7.0160901062526638E-3</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D154">
+        <v>16.3</v>
+      </c>
+      <c r="E154">
+        <v>82.99556372043071</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>15.3</v>
       </c>
@@ -2113,8 +3045,14 @@
       <c r="C155">
         <v>7.2746090539204727E-3</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D155">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E155">
+        <v>79.85580667351411</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>15.4</v>
       </c>
@@ -2124,8 +3062,14 @@
       <c r="C156">
         <v>7.6302287457325722E-3</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D156">
+        <v>16.5</v>
+      </c>
+      <c r="E156">
+        <v>82.068156037475049</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>15.5</v>
       </c>
@@ -2135,8 +3079,14 @@
       <c r="C157">
         <v>7.7520103634242509E-3</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D157">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E157">
+        <v>97.572897467846403</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>15.6</v>
       </c>
@@ -2146,8 +3096,14 @@
       <c r="C158">
         <v>8.1226210733424727E-3</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D158">
+        <v>16.7</v>
+      </c>
+      <c r="E158">
+        <v>107.36394588029253</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>15.7</v>
       </c>
@@ -2157,8 +3113,14 @@
       <c r="C159">
         <v>8.0515109410820313E-3</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D159">
+        <v>16.8</v>
+      </c>
+      <c r="E159">
+        <v>74.133253509289887</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>15.8</v>
       </c>
@@ -2168,8 +3130,14 @@
       <c r="C160">
         <v>8.4969043746389861E-3</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D160">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E160">
+        <v>75.378543725387942</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>15.9</v>
       </c>
@@ -2179,8 +3147,14 @@
       <c r="C161">
         <v>8.6886330577831145E-3</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D161">
+        <v>17</v>
+      </c>
+      <c r="E161">
+        <v>75.091909986237113</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>16</v>
       </c>
@@ -2190,8 +3164,14 @@
       <c r="C162">
         <v>8.9895987644790024E-3</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D162">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="E162">
+        <v>75.416452945133159</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>16.100000000000001</v>
       </c>
@@ -2201,8 +3181,14 @@
       <c r="C163">
         <v>9.4031035215539818E-3</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D163">
+        <v>17.2</v>
+      </c>
+      <c r="E163">
+        <v>75.744339832437333</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>16.2</v>
       </c>
@@ -2212,8 +3198,14 @@
       <c r="C164">
         <v>9.5510597228081057E-3</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D164">
+        <v>17.3</v>
+      </c>
+      <c r="E164">
+        <v>76.186964198464182</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>16.3</v>
       </c>
@@ -2223,8 +3215,14 @@
       <c r="C165">
         <v>9.6808551504404625E-3</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D165">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E165">
+        <v>71.512623135491808</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>16.399999999999999</v>
       </c>
@@ -2234,8 +3232,14 @@
       <c r="C166">
         <v>9.8112636391351864E-3</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D166">
+        <v>17.5</v>
+      </c>
+      <c r="E166">
+        <v>73.16147296748025</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>16.5</v>
       </c>
@@ -2245,8 +3249,14 @@
       <c r="C167">
         <v>9.9387386286148537E-3</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D167">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E167">
+        <v>85.454179856820602</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>16.600000000000001</v>
       </c>
@@ -2256,8 +3266,14 @@
       <c r="C168">
         <v>9.4933805365595425E-3</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D168">
+        <v>17.7</v>
+      </c>
+      <c r="E168">
+        <v>71.09949475872763</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>16.7</v>
       </c>
@@ -2267,8 +3283,14 @@
       <c r="C169">
         <v>9.3377460270605908E-3</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D169">
+        <v>17.8</v>
+      </c>
+      <c r="E169">
+        <v>44.742276491250813</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>16.8</v>
       </c>
@@ -2278,8 +3300,14 @@
       <c r="C170">
         <v>9.3323229377589249E-3</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D170">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="E170">
+        <v>50.162252617427448</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>16.899999999999999</v>
       </c>
@@ -2289,8 +3317,14 @@
       <c r="C171">
         <v>9.1049668932793246E-3</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D171">
+        <v>18</v>
+      </c>
+      <c r="E171">
+        <v>50.434801227358328</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>17</v>
       </c>
@@ -2300,8 +3334,14 @@
       <c r="C172">
         <v>9.2152483924748535E-3</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D172">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="E172">
+        <v>50.406419214488274</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>17.100000000000001</v>
       </c>
@@ -2311,8 +3351,14 @@
       <c r="C173">
         <v>9.1231749543808725E-3</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D173">
+        <v>18.2</v>
+      </c>
+      <c r="E173">
+        <v>49.775872861444732</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>17.2</v>
       </c>
@@ -2322,8 +3368,14 @@
       <c r="C174">
         <v>8.9575767436081144E-3</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D174">
+        <v>18.3</v>
+      </c>
+      <c r="E174">
+        <v>48.89440584789088</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>17.3</v>
       </c>
@@ -2333,8 +3385,14 @@
       <c r="C175">
         <v>9.0570874247412371E-3</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D175">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="E175">
+        <v>43.830518006629603</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>17.399999999999999</v>
       </c>
@@ -2344,8 +3402,14 @@
       <c r="C176">
         <v>9.1955887379092851E-3</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D176">
+        <v>18.5</v>
+      </c>
+      <c r="E176">
+        <v>43.830518006629603</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>17.5</v>
       </c>
@@ -2355,8 +3419,14 @@
       <c r="C177">
         <v>9.3355548164795205E-3</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D177">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E177">
+        <v>40.714883761226837</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>17.600000000000001</v>
       </c>
@@ -2366,8 +3436,14 @@
       <c r="C178">
         <v>9.8697859544836439E-3</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D178">
+        <v>18.7</v>
+      </c>
+      <c r="E178">
+        <v>26.14235993076684</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>17.7</v>
       </c>
@@ -2377,8 +3453,14 @@
       <c r="C179">
         <v>1.00043953167366E-2</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D179">
+        <v>18.8</v>
+      </c>
+      <c r="E179">
+        <v>24.217483109526469</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>17.8</v>
       </c>
@@ -2388,8 +3470,14 @@
       <c r="C180">
         <v>1.0610161222934469E-2</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D180">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E180">
+        <v>29.611067087183059</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>17.899999999999999</v>
       </c>
@@ -2399,8 +3487,14 @@
       <c r="C181">
         <v>1.088535716083595E-2</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D181">
+        <v>19</v>
+      </c>
+      <c r="E181">
+        <v>28.943679586413136</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>18</v>
       </c>
@@ -2410,8 +3504,14 @@
       <c r="C182">
         <v>1.149157974840744E-2</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D182">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E182">
+        <v>26.761418550149379</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>18.100000000000001</v>
       </c>
@@ -2421,8 +3521,14 @@
       <c r="C183">
         <v>1.199873898142626E-2</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D183">
+        <v>19.2</v>
+      </c>
+      <c r="E183">
+        <v>26.052445527892029</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>18.2</v>
       </c>
@@ -2432,8 +3538,14 @@
       <c r="C184">
         <v>1.235384392629587E-2</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D184">
+        <v>19.3</v>
+      </c>
+      <c r="E184">
+        <v>25.833089508754622</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>18.3</v>
       </c>
@@ -2443,8 +3555,14 @@
       <c r="C185">
         <v>1.3010741813368641E-2</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D185">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E185">
+        <v>21.67210799299928</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>18.399999999999999</v>
       </c>
@@ -2454,8 +3572,14 @@
       <c r="C186">
         <v>1.373268393191289E-2</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D186">
+        <v>19.5</v>
+      </c>
+      <c r="E186">
+        <v>23.136371857675066</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>18.5</v>
       </c>
@@ -2465,8 +3589,14 @@
       <c r="C187">
         <v>1.4443175786515329E-2</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D187">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E187">
+        <v>28.919200618427034</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>18.600000000000001</v>
       </c>
@@ -2476,8 +3606,14 @@
       <c r="C188">
         <v>1.4868565421953009E-2</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D188">
+        <v>19.7</v>
+      </c>
+      <c r="E188">
+        <v>34.636454545190595</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>18.7</v>
       </c>
@@ -2487,8 +3623,14 @@
       <c r="C189">
         <v>1.5687280643581249E-2</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D189">
+        <v>19.8</v>
+      </c>
+      <c r="E189">
+        <v>36.56802064510304</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>18.8</v>
       </c>
@@ -2498,8 +3640,14 @@
       <c r="C190">
         <v>1.6482023323892449E-2</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D190">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E190">
+        <v>40.994696885095991</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>18.899999999999999</v>
       </c>
@@ -2509,8 +3657,14 @@
       <c r="C191">
         <v>1.681592406845607E-2</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D191">
+        <v>20</v>
+      </c>
+      <c r="E191">
+        <v>39.815066017258999</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>19</v>
       </c>
@@ -2520,8 +3674,14 @@
       <c r="C192">
         <v>1.734497005949015E-2</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D192">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E192">
+        <v>38.840961341818556</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>19.100000000000001</v>
       </c>
@@ -2531,8 +3691,14 @@
       <c r="C193">
         <v>1.7997329922285778E-2</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D193">
+        <v>20.2</v>
+      </c>
+      <c r="E193">
+        <v>38.299196915164138</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>19.2</v>
       </c>
@@ -2542,8 +3708,14 @@
       <c r="C194">
         <v>1.8195411165135851E-2</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D194">
+        <v>20.3</v>
+      </c>
+      <c r="E194">
+        <v>37.756452472243772</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>19.3</v>
       </c>
@@ -2553,8 +3725,14 @@
       <c r="C195">
         <v>1.881890100288661E-2</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D195">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E195">
+        <v>35.714769737158235</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>19.399999999999999</v>
       </c>
@@ -2564,8 +3742,14 @@
       <c r="C196">
         <v>1.9431979255617869E-2</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D196">
+        <v>20.5</v>
+      </c>
+      <c r="E196">
+        <v>38.639097961698049</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>19.5</v>
       </c>
@@ -2575,8 +3759,14 @@
       <c r="C197">
         <v>1.992177124559338E-2</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D197">
+        <v>20.6</v>
+      </c>
+      <c r="E197">
+        <v>46.967112390020596</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>19.600000000000001</v>
       </c>
@@ -2586,8 +3776,14 @@
       <c r="C198">
         <v>2.0442534454331619E-2</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D198">
+        <v>20.7</v>
+      </c>
+      <c r="E198">
+        <v>54.192718968550736</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>19.7</v>
       </c>
@@ -2597,8 +3793,14 @@
       <c r="C199">
         <v>2.0453073063481458E-2</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D199">
+        <v>20.8</v>
+      </c>
+      <c r="E199">
+        <v>52.247979865988803</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>19.8</v>
       </c>
@@ -2608,8 +3810,14 @@
       <c r="C200">
         <v>2.1092395439124941E-2</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D200">
+        <v>20.9</v>
+      </c>
+      <c r="E200">
+        <v>54.924344223103482</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>19.899999999999999</v>
       </c>
@@ -2619,8 +3827,14 @@
       <c r="C201">
         <v>2.1220334015408699E-2</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D201">
+        <v>21</v>
+      </c>
+      <c r="E201">
+        <v>54.530923602930557</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>20</v>
       </c>
@@ -2630,8 +3844,14 @@
       <c r="C202">
         <v>2.1840867983036239E-2</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D202">
+        <v>21.1</v>
+      </c>
+      <c r="E202">
+        <v>54.010195885189702</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>20.100000000000001</v>
       </c>
@@ -2641,8 +3861,14 @@
       <c r="C203">
         <v>2.2142878735066759E-2</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D203">
+        <v>21.2</v>
+      </c>
+      <c r="E203">
+        <v>53.767989160611471</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>20.2</v>
       </c>
@@ -2652,8 +3878,14 @@
       <c r="C204">
         <v>2.2699724438389669E-2</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D204">
+        <v>21.3</v>
+      </c>
+      <c r="E204">
+        <v>54.659653709242619</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>20.3</v>
       </c>
@@ -2663,8 +3895,14 @@
       <c r="C205">
         <v>2.333070799042021E-2</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D205">
+        <v>21.4</v>
+      </c>
+      <c r="E205">
+        <v>52.74865131301722</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>20.399999999999999</v>
       </c>
@@ -2674,8 +3912,14 @@
       <c r="C206">
         <v>2.3615909799571969E-2</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D206">
+        <v>21.5</v>
+      </c>
+      <c r="E206">
+        <v>55.571004346637707</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>20.5</v>
       </c>
@@ -2685,8 +3929,14 @@
       <c r="C207">
         <v>2.433576131281601E-2</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D207">
+        <v>21.6</v>
+      </c>
+      <c r="E207">
+        <v>60.127827914354725</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>20.6</v>
       </c>
@@ -2696,8 +3946,14 @@
       <c r="C208">
         <v>2.4474160744422241E-2</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D208">
+        <v>21.7</v>
+      </c>
+      <c r="E208">
+        <v>57.588458190589975</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>20.7</v>
       </c>
@@ -2707,8 +3963,14 @@
       <c r="C209">
         <v>2.3872669599431979E-2</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D209">
+        <v>21.8</v>
+      </c>
+      <c r="E209">
+        <v>49.622536012507538</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>20.8</v>
       </c>
@@ -2718,8 +3980,14 @@
       <c r="C210">
         <v>2.430020457207966E-2</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D210">
+        <v>21.9</v>
+      </c>
+      <c r="E210">
+        <v>45.850021188305909</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>20.9</v>
       </c>
@@ -2729,8 +3997,14 @@
       <c r="C211">
         <v>2.502868274065213E-2</v>
       </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D211">
+        <v>22</v>
+      </c>
+      <c r="E211">
+        <v>41.242090731278786</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>21</v>
       </c>
@@ -2740,8 +4014,14 @@
       <c r="C212">
         <v>2.571590584670054E-2</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D212">
+        <v>22.1</v>
+      </c>
+      <c r="E212">
+        <v>38.747696284589011</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>21.1</v>
       </c>
@@ -2751,8 +4031,14 @@
       <c r="C213">
         <v>2.6427010434337199E-2</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D213">
+        <v>22.2</v>
+      </c>
+      <c r="E213">
+        <v>37.698221215426081</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>21.2</v>
       </c>
@@ -2762,8 +4048,14 @@
       <c r="C214">
         <v>2.7164426095724239E-2</v>
       </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D214">
+        <v>22.3</v>
+      </c>
+      <c r="E214">
+        <v>37.477568206116786</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>21.3</v>
       </c>
@@ -2773,8 +4065,14 @@
       <c r="C215">
         <v>2.8158183215137449E-2</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D215">
+        <v>22.4</v>
+      </c>
+      <c r="E215">
+        <v>36.59485292714178</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>21.4</v>
       </c>
@@ -2784,8 +4082,14 @@
       <c r="C216">
         <v>2.910869962355369E-2</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D216">
+        <v>22.5</v>
+      </c>
+      <c r="E216">
+        <v>38.852185024413124</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>21.5</v>
       </c>
@@ -2795,8 +4099,14 @@
       <c r="C217">
         <v>2.9795444020981918E-2</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D217">
+        <v>22.6</v>
+      </c>
+      <c r="E217">
+        <v>40.633608236931785</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>21.6</v>
       </c>
@@ -2806,8 +4116,14 @@
       <c r="C218">
         <v>3.0228185840321529E-2</v>
       </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D218">
+        <v>22.7</v>
+      </c>
+      <c r="E218">
+        <v>35.018215002009839</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>21.7</v>
       </c>
@@ -2817,8 +4133,14 @@
       <c r="C219">
         <v>2.999453332486169E-2</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D219">
+        <v>22.8</v>
+      </c>
+      <c r="E219">
+        <v>27.765306432776253</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>21.8</v>
       </c>
@@ -2828,8 +4150,14 @@
       <c r="C220">
         <v>3.0658095919356861E-2</v>
       </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D220">
+        <v>22.9</v>
+      </c>
+      <c r="E220">
+        <v>27.106239704475705</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>21.9</v>
       </c>
@@ -2839,8 +4167,14 @@
       <c r="C221">
         <v>3.1829429421893152E-2</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D221">
+        <v>23</v>
+      </c>
+      <c r="E221">
+        <v>31.732078040992203</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>22</v>
       </c>
@@ -2850,8 +4184,14 @@
       <c r="C222">
         <v>3.4140697101972137E-2</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D222">
+        <v>23.1</v>
+      </c>
+      <c r="E222">
+        <v>35.997359467669895</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>22.1</v>
       </c>
@@ -2861,8 +4201,14 @@
       <c r="C223">
         <v>3.5524488552135983E-2</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D223">
+        <v>23.2</v>
+      </c>
+      <c r="E223">
+        <v>38.539374691557924</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>22.2</v>
       </c>
@@ -2872,8 +4218,14 @@
       <c r="C224">
         <v>3.6637526596844203E-2</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D224">
+        <v>23.3</v>
+      </c>
+      <c r="E224">
+        <v>39.817697377411776</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>22.3</v>
       </c>
@@ -2883,8 +4235,14 @@
       <c r="C225">
         <v>3.7263702737356602E-2</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D225">
+        <v>23.4</v>
+      </c>
+      <c r="E225">
+        <v>38.834959259463965</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>22.4</v>
       </c>
@@ -2894,8 +4252,14 @@
       <c r="C226">
         <v>3.7798380379557427E-2</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D226">
+        <v>23.5</v>
+      </c>
+      <c r="E226">
+        <v>42.787186320021753</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>22.5</v>
       </c>
@@ -2905,8 +4269,14 @@
       <c r="C227">
         <v>3.8200292516264257E-2</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D227">
+        <v>23.6</v>
+      </c>
+      <c r="E227">
+        <v>48.800541147397304</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>22.6</v>
       </c>
@@ -2916,8 +4286,14 @@
       <c r="C228">
         <v>3.7008170245475272E-2</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D228">
+        <v>23.7</v>
+      </c>
+      <c r="E228">
+        <v>51.922242460778534</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>22.7</v>
       </c>
@@ -2927,8 +4303,14 @@
       <c r="C229">
         <v>3.7368518533452279E-2</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D229">
+        <v>23.8</v>
+      </c>
+      <c r="E229">
+        <v>59.027336228925947</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>22.8</v>
       </c>
@@ -2938,8 +4320,14 @@
       <c r="C230">
         <v>3.8396994118489389E-2</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D230">
+        <v>23.9</v>
+      </c>
+      <c r="E230">
+        <v>65.492182867862397</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>22.9</v>
       </c>
@@ -2949,8 +4337,14 @@
       <c r="C231">
         <v>3.8288899868713408E-2</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D231">
+        <v>24</v>
+      </c>
+      <c r="E231">
+        <v>67.572853209063211</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>23</v>
       </c>
@@ -2960,8 +4354,14 @@
       <c r="C232">
         <v>3.772483172761773E-2</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D232">
+        <v>24.1</v>
+      </c>
+      <c r="E232">
+        <v>69.313409483635098</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>23.1</v>
       </c>
@@ -2971,8 +4371,14 @@
       <c r="C233">
         <v>3.7245973521103599E-2</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D233">
+        <v>24.2</v>
+      </c>
+      <c r="E233">
+        <v>71.451529779715571</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>23.2</v>
       </c>
@@ -2982,8 +4388,14 @@
       <c r="C234">
         <v>3.6685991873996182E-2</v>
       </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D234">
+        <v>24.3</v>
+      </c>
+      <c r="E234">
+        <v>73.812073064560366</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>23.3</v>
       </c>
@@ -2993,8 +4405,14 @@
       <c r="C235">
         <v>3.5984103830795117E-2</v>
       </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D235">
+        <v>24.4</v>
+      </c>
+      <c r="E235">
+        <v>76.842913135769692</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>23.4</v>
       </c>
@@ -3004,8 +4422,14 @@
       <c r="C236">
         <v>3.5462625563169273E-2</v>
       </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D236">
+        <v>24.5</v>
+      </c>
+      <c r="E236">
+        <v>83.786641053180489</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>23.5</v>
       </c>
@@ -3015,8 +4439,14 @@
       <c r="C237">
         <v>3.4790302373299893E-2</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D237">
+        <v>24.6</v>
+      </c>
+      <c r="E237">
+        <v>86.89551734252133</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>23.6</v>
       </c>
@@ -3026,8 +4456,14 @@
       <c r="C238">
         <v>3.2433252980364993E-2</v>
       </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D238">
+        <v>24.7</v>
+      </c>
+      <c r="E238">
+        <v>86.187267130979492</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>23.7</v>
       </c>
@@ -3037,8 +4473,14 @@
       <c r="C239">
         <v>3.038312796999321E-2</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D239">
+        <v>24.8</v>
+      </c>
+      <c r="E239">
+        <v>83.664665596335439</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>23.8</v>
       </c>
@@ -3048,8 +4490,14 @@
       <c r="C240">
         <v>2.8345371479740492E-2</v>
       </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D240">
+        <v>24.9</v>
+      </c>
+      <c r="E240">
+        <v>80.627087139763674</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>23.9</v>
       </c>
@@ -3059,8 +4507,14 @@
       <c r="C241">
         <v>2.7323588154987598E-2</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D241">
+        <v>25</v>
+      </c>
+      <c r="E241">
+        <v>80.09863981003879</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>24</v>
       </c>
@@ -3071,7 +4525,7 @@
         <v>2.680167245975492E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>24.1</v>
       </c>
@@ -3082,7 +4536,7 @@
         <v>2.6043842199607731E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>24.2</v>
       </c>
@@ -3093,7 +4547,7 @@
         <v>2.5427017880527071E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>24.3</v>
       </c>
@@ -3104,7 +4558,7 @@
         <v>2.503648375140774E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>24.4</v>
       </c>
@@ -3115,7 +4569,7 @@
         <v>2.4279144879683551E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>24.5</v>
       </c>
@@ -3126,7 +4580,7 @@
         <v>2.3267498120673521E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>24.6</v>
       </c>
@@ -3137,7 +4591,7 @@
         <v>2.227970858789741E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>24.7</v>
       </c>
@@ -3148,7 +4602,7 @@
         <v>2.1242659023816359E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>24.8</v>
       </c>
@@ -3159,7 +4613,7 @@
         <v>2.0473676037175141E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>24.9</v>
       </c>
@@ -3170,7 +4624,7 @@
         <v>1.971590617715856E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>25</v>
       </c>

</xml_diff>